<commit_message>
Add code and forest plots
</commit_message>
<xml_diff>
--- a/data/data_extraction_te_20230205.xlsx
+++ b/data/data_extraction_te_20230205.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26322"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared Documents/General/ONLINE PARENTING SR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F81CF18-4364-4706-ACB8-D46616F23D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63139E54-54C8-4B28-9D25-58140888C2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="466">
   <si>
     <t>study</t>
   </si>
@@ -1472,13 +1472,13 @@
     <t>Positive behavior in infant interaction</t>
   </si>
   <si>
-    <t>Infant positive behavior</t>
+    <t>Infant behavior</t>
   </si>
   <si>
     <t>Parent responsiveness in infant interaction</t>
   </si>
   <si>
-    <t>Parent responsiveness</t>
+    <t>Responsiveness</t>
   </si>
   <si>
     <t>https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FBreitenstein%20%282021%29%20A%20Randomized%20Trial%20of%20Digitally%20Delivered%2C%20Self%2DAdministered%20Parent%20Training%20in%20Primary%20Care%2D%20Effects%20on%20Parenting%20and%20Child%20Behavior%2Epdf&amp;q=Breitenstein&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR&amp;parentview=7</t>
@@ -1532,7 +1532,7 @@
     <t>Parenting stress - parent-child domain</t>
   </si>
   <si>
-    <t>Parent-child domain</t>
+    <t>Dyadic domain</t>
   </si>
   <si>
     <t>Parenting stress - child domain</t>
@@ -1544,13 +1544,22 @@
     <t>https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FEhrenseft%20%282016%29%20Web%2DBased%20Prevention%20of%20Parenting%20Difficulties%20in%20Young%2C%20Urban%20Mothers%20Enrolled%20in%20Post%2DSecondary%20Education%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL</t>
   </si>
   <si>
+    <t>O365-MERTIL - Online Parenting SR &amp; Protocol - Lennard (2021) Randomized controlled trial of a brief online self-compassion intervention for mothers of infants- Effects on mental health outcomes.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
     <t>Post-traumatic</t>
   </si>
   <si>
+    <t>O365-MERTIL - Online Parenting SR &amp; Protocol - Lindsay (2017) The effectiveness of universal parenting programmes- the CANparent trial.pdf - All Documents (sharepoint.com)</t>
+  </si>
+  <si>
     <t>Stress frequency</t>
   </si>
   <si>
     <t>Stress intensity</t>
+  </si>
+  <si>
+    <t>O365-MERTIL - Online Parenting SR &amp; Protocol - Matvienko-Sikar (2017) Effects of a novel positive psychological intervention on prenatal stress and well-being- A pilot randomised controlled trial.pdf - All Documents (sharepoint.com)</t>
   </si>
   <si>
     <t>Parenting stress index - competence</t>
@@ -1691,7 +1700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1722,7 +1731,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7647,8 +7655,8 @@
   <dimension ref="A1:AS140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I71" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T91" sqref="T91"/>
+      <pane xSplit="1" topLeftCell="B94" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7776,7 +7784,7 @@
       <c r="AQ1" s="9"/>
     </row>
     <row r="2" spans="1:45">
-      <c r="A2" s="20" t="s">
+      <c r="A2" t="s">
         <v>193</v>
       </c>
       <c r="B2" t="s">
@@ -7845,7 +7853,7 @@
       <c r="AS2" s="2"/>
     </row>
     <row r="3" spans="1:45">
-      <c r="A3" s="20" t="s">
+      <c r="A3" t="s">
         <v>193</v>
       </c>
       <c r="B3" t="s">
@@ -7914,7 +7922,7 @@
       <c r="AS3" s="2"/>
     </row>
     <row r="4" spans="1:45">
-      <c r="A4" s="20" t="s">
+      <c r="A4" t="s">
         <v>194</v>
       </c>
       <c r="B4" t="s">
@@ -8001,7 +8009,7 @@
       <c r="AS4" s="2"/>
     </row>
     <row r="5" spans="1:45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" t="s">
         <v>194</v>
       </c>
       <c r="B5" t="s">
@@ -8551,7 +8559,7 @@
       </c>
     </row>
     <row r="12" spans="1:45">
-      <c r="A12" s="20" t="s">
+      <c r="A12" t="s">
         <v>196</v>
       </c>
       <c r="B12" t="s">
@@ -8622,7 +8630,7 @@
       <c r="AS12" s="2"/>
     </row>
     <row r="13" spans="1:45">
-      <c r="A13" s="20" t="s">
+      <c r="A13" t="s">
         <v>196</v>
       </c>
       <c r="B13" t="s">
@@ -8886,7 +8894,7 @@
       </c>
     </row>
     <row r="17" spans="1:45">
-      <c r="A17" s="20" t="s">
+      <c r="A17" t="s">
         <v>197</v>
       </c>
       <c r="B17" t="s">
@@ -8970,7 +8978,7 @@
       <c r="AS17" s="2"/>
     </row>
     <row r="18" spans="1:45">
-      <c r="A18" s="20" t="s">
+      <c r="A18" t="s">
         <v>197</v>
       </c>
       <c r="B18" t="s">
@@ -9054,7 +9062,7 @@
       <c r="AS18" s="2"/>
     </row>
     <row r="19" spans="1:45">
-      <c r="A19" s="20" t="s">
+      <c r="A19" t="s">
         <v>197</v>
       </c>
       <c r="B19" t="s">
@@ -9138,7 +9146,7 @@
       <c r="AS19" s="2"/>
     </row>
     <row r="20" spans="1:45">
-      <c r="A20" s="20" t="s">
+      <c r="A20" t="s">
         <v>197</v>
       </c>
       <c r="B20" t="s">
@@ -9222,7 +9230,7 @@
       <c r="AS20" s="2"/>
     </row>
     <row r="21" spans="1:45">
-      <c r="A21" s="20" t="s">
+      <c r="A21" t="s">
         <v>197</v>
       </c>
       <c r="B21" t="s">
@@ -9385,7 +9393,7 @@
       </c>
     </row>
     <row r="23" spans="1:45">
-      <c r="A23" s="20" t="s">
+      <c r="A23" t="s">
         <v>193</v>
       </c>
       <c r="B23" t="s">
@@ -9451,7 +9459,7 @@
       <c r="AS23" s="2"/>
     </row>
     <row r="24" spans="1:45">
-      <c r="A24" s="20" t="s">
+      <c r="A24" t="s">
         <v>194</v>
       </c>
       <c r="B24" t="s">
@@ -9538,7 +9546,7 @@
       <c r="AS24" s="2"/>
     </row>
     <row r="25" spans="1:45">
-      <c r="A25" s="20" t="s">
+      <c r="A25" t="s">
         <v>194</v>
       </c>
       <c r="B25" t="s">
@@ -9625,7 +9633,7 @@
       <c r="AS25" s="2"/>
     </row>
     <row r="26" spans="1:45">
-      <c r="A26" s="20" t="s">
+      <c r="A26" t="s">
         <v>57</v>
       </c>
       <c r="C26">
@@ -9688,7 +9696,7 @@
       </c>
     </row>
     <row r="27" spans="1:45">
-      <c r="A27" s="20" t="s">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
       <c r="C27">
@@ -9751,7 +9759,7 @@
       </c>
     </row>
     <row r="28" spans="1:45">
-      <c r="A28" s="20" t="s">
+      <c r="A28" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -9833,7 +9841,7 @@
       </c>
     </row>
     <row r="29" spans="1:45">
-      <c r="A29" s="20" t="s">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -9915,7 +9923,7 @@
       </c>
     </row>
     <row r="30" spans="1:45">
-      <c r="A30" s="20" t="s">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -9997,7 +10005,7 @@
       </c>
     </row>
     <row r="31" spans="1:45">
-      <c r="A31" s="20" t="s">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
       <c r="C31">
@@ -10060,7 +10068,7 @@
       </c>
     </row>
     <row r="32" spans="1:45">
-      <c r="A32" s="20" t="s">
+      <c r="A32" t="s">
         <v>71</v>
       </c>
       <c r="C32">
@@ -10123,7 +10131,7 @@
       </c>
     </row>
     <row r="33" spans="1:45">
-      <c r="A33" s="20" t="s">
+      <c r="A33" t="s">
         <v>196</v>
       </c>
       <c r="B33" t="s">
@@ -10192,7 +10200,7 @@
       <c r="AS33" s="2"/>
     </row>
     <row r="34" spans="1:45">
-      <c r="A34" s="20" t="s">
+      <c r="A34" t="s">
         <v>196</v>
       </c>
       <c r="B34" t="s">
@@ -10261,7 +10269,7 @@
       <c r="AS34" s="2"/>
     </row>
     <row r="35" spans="1:45">
-      <c r="A35" s="20" t="s">
+      <c r="A35" t="s">
         <v>76</v>
       </c>
       <c r="C35">
@@ -10324,7 +10332,7 @@
       </c>
     </row>
     <row r="36" spans="1:45">
-      <c r="A36" s="20" t="s">
+      <c r="A36" t="s">
         <v>76</v>
       </c>
       <c r="C36">
@@ -10387,7 +10395,7 @@
       </c>
     </row>
     <row r="37" spans="1:45">
-      <c r="A37" s="20" t="s">
+      <c r="A37" t="s">
         <v>76</v>
       </c>
       <c r="C37">
@@ -10450,7 +10458,7 @@
       </c>
     </row>
     <row r="38" spans="1:45">
-      <c r="A38" s="20" t="s">
+      <c r="A38" t="s">
         <v>76</v>
       </c>
       <c r="C38">
@@ -10513,7 +10521,7 @@
       </c>
     </row>
     <row r="39" spans="1:45">
-      <c r="A39" s="20" t="s">
+      <c r="A39" t="s">
         <v>83</v>
       </c>
       <c r="C39">
@@ -10579,7 +10587,7 @@
       </c>
     </row>
     <row r="40" spans="1:45">
-      <c r="A40" s="20" t="s">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
       <c r="C40">
@@ -10644,7 +10652,7 @@
       </c>
     </row>
     <row r="41" spans="1:45">
-      <c r="A41" s="20" t="s">
+      <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="C41">
@@ -10709,7 +10717,7 @@
       </c>
     </row>
     <row r="42" spans="1:45">
-      <c r="A42" s="20" t="s">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
       <c r="C42">
@@ -10774,7 +10782,7 @@
       </c>
     </row>
     <row r="43" spans="1:45">
-      <c r="A43" s="20" t="s">
+      <c r="A43" t="s">
         <v>197</v>
       </c>
       <c r="B43" t="s">
@@ -10858,7 +10866,7 @@
       <c r="AS43" s="2"/>
     </row>
     <row r="44" spans="1:45">
-      <c r="A44" s="20" t="s">
+      <c r="A44" t="s">
         <v>197</v>
       </c>
       <c r="B44" t="s">
@@ -10942,7 +10950,7 @@
       <c r="AS44" s="2"/>
     </row>
     <row r="45" spans="1:45">
-      <c r="A45" s="20" t="s">
+      <c r="A45" t="s">
         <v>197</v>
       </c>
       <c r="B45" t="s">
@@ -11026,7 +11034,7 @@
       <c r="AS45" s="2"/>
     </row>
     <row r="46" spans="1:45">
-      <c r="A46" s="20" t="s">
+      <c r="A46" t="s">
         <v>197</v>
       </c>
       <c r="B46" t="s">
@@ -11110,7 +11118,7 @@
       <c r="AS46" s="2"/>
     </row>
     <row r="47" spans="1:45">
-      <c r="A47" s="20" t="s">
+      <c r="A47" t="s">
         <v>197</v>
       </c>
       <c r="B47" t="s">
@@ -11194,7 +11202,7 @@
       <c r="AS47" s="2"/>
     </row>
     <row r="48" spans="1:45">
-      <c r="A48" s="20" t="s">
+      <c r="A48" t="s">
         <v>200</v>
       </c>
       <c r="B48" t="s">
@@ -11278,7 +11286,7 @@
       <c r="AS48" s="2"/>
     </row>
     <row r="49" spans="1:45">
-      <c r="A49" s="20" t="s">
+      <c r="A49" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -11347,7 +11355,7 @@
       </c>
     </row>
     <row r="50" spans="1:45">
-      <c r="A50" s="20" t="s">
+      <c r="A50" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -11416,7 +11424,7 @@
       </c>
     </row>
     <row r="51" spans="1:45">
-      <c r="A51" s="20" t="s">
+      <c r="A51" t="s">
         <v>111</v>
       </c>
       <c r="C51">
@@ -11482,7 +11490,7 @@
       </c>
     </row>
     <row r="52" spans="1:45">
-      <c r="A52" s="20" t="s">
+      <c r="A52" t="s">
         <v>76</v>
       </c>
       <c r="C52">
@@ -11545,7 +11553,7 @@
       </c>
     </row>
     <row r="53" spans="1:45">
-      <c r="A53" s="20" t="s">
+      <c r="A53" t="s">
         <v>76</v>
       </c>
       <c r="C53">
@@ -11608,7 +11616,7 @@
       </c>
     </row>
     <row r="54" spans="1:45">
-      <c r="A54" s="20" t="s">
+      <c r="A54" t="s">
         <v>76</v>
       </c>
       <c r="C54">
@@ -11671,7 +11679,7 @@
       </c>
     </row>
     <row r="55" spans="1:45">
-      <c r="A55" s="20" t="s">
+      <c r="A55" t="s">
         <v>76</v>
       </c>
       <c r="C55">
@@ -11734,7 +11742,7 @@
       </c>
     </row>
     <row r="56" spans="1:45">
-      <c r="A56" s="20" t="s">
+      <c r="A56" t="s">
         <v>83</v>
       </c>
       <c r="C56">
@@ -11792,7 +11800,7 @@
       </c>
     </row>
     <row r="57" spans="1:45">
-      <c r="A57" s="20" t="s">
+      <c r="A57" t="s">
         <v>45</v>
       </c>
       <c r="C57">
@@ -11855,7 +11863,7 @@
       </c>
     </row>
     <row r="58" spans="1:45">
-      <c r="A58" s="20" t="s">
+      <c r="A58" t="s">
         <v>45</v>
       </c>
       <c r="C58">
@@ -11918,7 +11926,7 @@
       </c>
     </row>
     <row r="59" spans="1:45">
-      <c r="A59" s="20" t="s">
+      <c r="A59" t="s">
         <v>45</v>
       </c>
       <c r="C59">
@@ -11981,7 +11989,7 @@
       </c>
     </row>
     <row r="60" spans="1:45">
-      <c r="A60" s="20" t="s">
+      <c r="A60" t="s">
         <v>92</v>
       </c>
       <c r="C60">
@@ -12039,7 +12047,7 @@
       </c>
     </row>
     <row r="61" spans="1:45">
-      <c r="A61" s="20" t="s">
+      <c r="A61" t="s">
         <v>92</v>
       </c>
       <c r="C61">
@@ -12097,7 +12105,7 @@
       </c>
     </row>
     <row r="62" spans="1:45">
-      <c r="A62" s="20" t="s">
+      <c r="A62" t="s">
         <v>92</v>
       </c>
       <c r="C62">
@@ -12155,7 +12163,7 @@
       </c>
     </row>
     <row r="63" spans="1:45">
-      <c r="A63" s="20" t="s">
+      <c r="A63" t="s">
         <v>194</v>
       </c>
       <c r="B63" t="s">
@@ -12242,7 +12250,7 @@
       <c r="AS63" s="2"/>
     </row>
     <row r="64" spans="1:45">
-      <c r="A64" s="20" t="s">
+      <c r="A64" t="s">
         <v>194</v>
       </c>
       <c r="B64" t="s">
@@ -12329,7 +12337,7 @@
       <c r="AS64" s="2"/>
     </row>
     <row r="65" spans="1:45">
-      <c r="A65" s="20" t="s">
+      <c r="A65" t="s">
         <v>57</v>
       </c>
       <c r="C65">
@@ -12387,7 +12395,7 @@
       </c>
     </row>
     <row r="66" spans="1:45">
-      <c r="A66" s="20" t="s">
+      <c r="A66" t="s">
         <v>57</v>
       </c>
       <c r="C66">
@@ -12445,7 +12453,7 @@
       </c>
     </row>
     <row r="67" spans="1:45">
-      <c r="A67" s="20" t="s">
+      <c r="A67" t="s">
         <v>21</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -12523,7 +12531,7 @@
       </c>
     </row>
     <row r="68" spans="1:45">
-      <c r="A68" s="20" t="s">
+      <c r="A68" t="s">
         <v>21</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -12601,7 +12609,7 @@
       </c>
     </row>
     <row r="69" spans="1:45">
-      <c r="A69" s="20" t="s">
+      <c r="A69" t="s">
         <v>21</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -12679,7 +12687,7 @@
       </c>
     </row>
     <row r="70" spans="1:45">
-      <c r="A70" s="20" t="s">
+      <c r="A70" t="s">
         <v>111</v>
       </c>
       <c r="C70">
@@ -12737,7 +12745,7 @@
       </c>
     </row>
     <row r="71" spans="1:45">
-      <c r="A71" s="20" t="s">
+      <c r="A71" t="s">
         <v>149</v>
       </c>
       <c r="C71">
@@ -12795,7 +12803,7 @@
       </c>
     </row>
     <row r="72" spans="1:45">
-      <c r="A72" s="20" t="s">
+      <c r="A72" t="s">
         <v>149</v>
       </c>
       <c r="C72">
@@ -12853,7 +12861,7 @@
       </c>
     </row>
     <row r="73" spans="1:45">
-      <c r="A73" s="20" t="s">
+      <c r="A73" t="s">
         <v>83</v>
       </c>
       <c r="C73">
@@ -12911,7 +12919,7 @@
       </c>
     </row>
     <row r="74" spans="1:45">
-      <c r="A74" s="20" t="s">
+      <c r="A74" t="s">
         <v>45</v>
       </c>
       <c r="C74">
@@ -12974,7 +12982,7 @@
       </c>
     </row>
     <row r="75" spans="1:45">
-      <c r="A75" s="20" t="s">
+      <c r="A75" t="s">
         <v>45</v>
       </c>
       <c r="C75">
@@ -13037,7 +13045,7 @@
       </c>
     </row>
     <row r="76" spans="1:45">
-      <c r="A76" s="20" t="s">
+      <c r="A76" t="s">
         <v>45</v>
       </c>
       <c r="C76">
@@ -13100,7 +13108,7 @@
       </c>
     </row>
     <row r="77" spans="1:45">
-      <c r="A77" s="20" t="s">
+      <c r="A77" t="s">
         <v>202</v>
       </c>
       <c r="B77" t="s">
@@ -13184,7 +13192,7 @@
       <c r="AS77" s="2"/>
     </row>
     <row r="78" spans="1:45">
-      <c r="A78" s="20" t="s">
+      <c r="A78" t="s">
         <v>202</v>
       </c>
       <c r="B78" t="s">
@@ -13268,7 +13276,7 @@
       <c r="AS78" s="2"/>
     </row>
     <row r="79" spans="1:45">
-      <c r="A79" s="20" t="s">
+      <c r="A79" t="s">
         <v>178</v>
       </c>
       <c r="B79" t="s">
@@ -13356,7 +13364,7 @@
       <c r="AS79" s="2"/>
     </row>
     <row r="80" spans="1:45">
-      <c r="A80" s="20" t="s">
+      <c r="A80" t="s">
         <v>181</v>
       </c>
       <c r="B80" s="13" t="s">
@@ -13425,7 +13433,7 @@
       <c r="AS80" s="2"/>
     </row>
     <row r="81" spans="1:45">
-      <c r="A81" s="20" t="s">
+      <c r="A81" t="s">
         <v>181</v>
       </c>
       <c r="B81" t="s">
@@ -13494,7 +13502,7 @@
       <c r="AS81" s="2"/>
     </row>
     <row r="82" spans="1:45">
-      <c r="A82" s="20" t="s">
+      <c r="A82" t="s">
         <v>164</v>
       </c>
       <c r="B82" t="s">
@@ -13578,7 +13586,7 @@
       <c r="AS82" s="2"/>
     </row>
     <row r="83" spans="1:45">
-      <c r="A83" s="20" t="s">
+      <c r="A83" t="s">
         <v>164</v>
       </c>
       <c r="B83" t="s">
@@ -13662,7 +13670,7 @@
       <c r="AS83" s="2"/>
     </row>
     <row r="84" spans="1:45">
-      <c r="A84" s="20" t="s">
+      <c r="A84" t="s">
         <v>164</v>
       </c>
       <c r="B84" t="s">
@@ -13746,11 +13754,14 @@
       <c r="AS84" s="2"/>
     </row>
     <row r="85" spans="1:45">
-      <c r="A85" s="20" t="s">
+      <c r="A85" t="s">
         <v>51</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>417</v>
+      </c>
+      <c r="C85">
+        <v>84</v>
       </c>
       <c r="D85" t="s">
         <v>22</v>
@@ -13830,11 +13841,14 @@
       <c r="AS85" s="2"/>
     </row>
     <row r="86" spans="1:45">
-      <c r="A86" s="20" t="s">
+      <c r="A86" t="s">
         <v>51</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>417</v>
+      </c>
+      <c r="C86">
+        <v>85</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
@@ -13914,11 +13928,14 @@
       <c r="AS86" s="2"/>
     </row>
     <row r="87" spans="1:45">
-      <c r="A87" s="20" t="s">
+      <c r="A87" t="s">
         <v>92</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>422</v>
+      </c>
+      <c r="C87">
+        <v>86</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -13984,16 +14001,19 @@
         <f>IF(ISBLANK(I87), T87, SQRT(T87 ^ 2 / R87 + N87 ^ 2 / L87))</f>
         <v>0.7154099868434618</v>
       </c>
-      <c r="AC87" s="20" t="b">
+      <c r="AC87" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:45">
-      <c r="A88" s="20" t="s">
+      <c r="A88" t="s">
         <v>92</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>422</v>
+      </c>
+      <c r="C88">
+        <v>87</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -14059,16 +14079,19 @@
         <f>IF(ISBLANK(I88), T88, SQRT(T88 ^ 2 / R88 + N88 ^ 2 / L88))</f>
         <v>0.78466582329708146</v>
       </c>
-      <c r="AC88" s="20" t="b">
+      <c r="AC88" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:45">
-      <c r="A89" s="20" t="s">
+      <c r="A89" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>422</v>
+      </c>
+      <c r="C89">
+        <v>88</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -14134,16 +14157,19 @@
         <f>IF(ISBLANK(I89), T89, SQRT(T89 ^ 2 / R89 + N89 ^ 2 / L89))</f>
         <v>0.73662257154646438</v>
       </c>
-      <c r="AC89" s="20" t="b">
+      <c r="AC89" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:45">
-      <c r="A90" s="20" t="s">
+      <c r="A90" t="s">
         <v>103</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>424</v>
+      </c>
+      <c r="C90">
+        <v>89</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -14191,16 +14217,19 @@
         <f>IF(ISBLANK(I90), T90, SQRT(T90 ^ 2 / R90 + N90 ^ 2 / L90))</f>
         <v>6.38</v>
       </c>
-      <c r="AC90" s="20" t="b">
+      <c r="AC90" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:45">
-      <c r="A91" s="20" t="s">
+      <c r="A91" t="s">
         <v>196</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>426</v>
+      </c>
+      <c r="C91">
+        <v>90</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
@@ -14251,16 +14280,19 @@
       <c r="Z91">
         <v>2.1061696312518918E-2</v>
       </c>
-      <c r="AC91" s="20" t="b">
+      <c r="AC91" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:45">
-      <c r="A92" s="20" t="s">
+      <c r="A92" t="s">
         <v>196</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>426</v>
+      </c>
+      <c r="C92">
+        <v>91</v>
       </c>
       <c r="D92" t="s">
         <v>22</v>
@@ -14311,16 +14343,19 @@
       <c r="Z92">
         <v>2.6171741361614778E-2</v>
       </c>
-      <c r="AC92" s="20" t="b">
+      <c r="AC92" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:45">
-      <c r="A93" s="20" t="s">
+      <c r="A93" t="s">
         <v>186</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>428</v>
+      </c>
+      <c r="C93">
+        <v>92</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -14379,12 +14414,15 @@
       </c>
     </row>
     <row r="94" spans="1:45">
-      <c r="A94" s="20" t="s">
+      <c r="A94" t="s">
         <v>429</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>430</v>
       </c>
+      <c r="C94">
+        <v>93</v>
+      </c>
       <c r="D94" t="s">
         <v>22</v>
       </c>
@@ -14393,9 +14431,6 @@
       </c>
       <c r="F94" t="s">
         <v>338</v>
-      </c>
-      <c r="G94" t="s">
-        <v>431</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -14434,19 +14469,19 @@
       <c r="Z94">
         <v>0.16600000000000001</v>
       </c>
-      <c r="AC94" s="20" t="b">
+      <c r="AC94" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:45">
-      <c r="A95" s="20" t="s">
+      <c r="A95" t="s">
         <v>194</v>
       </c>
       <c r="B95" t="s">
         <v>400</v>
       </c>
       <c r="C95">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -14520,14 +14555,14 @@
       </c>
     </row>
     <row r="96" spans="1:45">
-      <c r="A96" s="20" t="s">
+      <c r="A96" t="s">
         <v>194</v>
       </c>
       <c r="B96" t="s">
         <v>400</v>
       </c>
       <c r="C96">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -14601,11 +14636,11 @@
       </c>
     </row>
     <row r="97" spans="1:45">
-      <c r="A97" s="20" t="s">
+      <c r="A97" t="s">
         <v>57</v>
       </c>
       <c r="C97">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -14659,11 +14694,11 @@
       </c>
     </row>
     <row r="98" spans="1:45">
-      <c r="A98" s="20" t="s">
+      <c r="A98" t="s">
         <v>57</v>
       </c>
       <c r="C98">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -14716,14 +14751,14 @@
       </c>
     </row>
     <row r="99" spans="1:45">
-      <c r="A99" s="20" t="s">
+      <c r="A99" t="s">
         <v>21</v>
       </c>
       <c r="B99" s="16" t="s">
         <v>406</v>
       </c>
       <c r="C99">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -14794,14 +14829,14 @@
       </c>
     </row>
     <row r="100" spans="1:45">
-      <c r="A100" s="20" t="s">
+      <c r="A100" t="s">
         <v>21</v>
       </c>
       <c r="B100" s="16" t="s">
         <v>406</v>
       </c>
       <c r="C100">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -14872,14 +14907,14 @@
       </c>
     </row>
     <row r="101" spans="1:45">
-      <c r="A101" s="20" t="s">
+      <c r="A101" t="s">
         <v>21</v>
       </c>
       <c r="B101" s="16" t="s">
         <v>406</v>
       </c>
       <c r="C101">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -14950,14 +14985,14 @@
       </c>
     </row>
     <row r="102" spans="1:45">
-      <c r="A102" s="20" t="s">
+      <c r="A102" t="s">
         <v>164</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C102">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D102" t="s">
         <v>22</v>
@@ -15035,14 +15070,14 @@
       </c>
     </row>
     <row r="103" spans="1:45">
-      <c r="A103" s="20" t="s">
+      <c r="A103" t="s">
         <v>164</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C103">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -15126,14 +15161,14 @@
       <c r="AS103" s="2"/>
     </row>
     <row r="104" spans="1:45">
-      <c r="A104" s="20" t="s">
+      <c r="A104" t="s">
         <v>164</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C104">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -15217,14 +15252,14 @@
       <c r="AS104" s="2"/>
     </row>
     <row r="105" spans="1:45">
-      <c r="A105" s="20" t="s">
+      <c r="A105" t="s">
         <v>164</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C105">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D105" t="s">
         <v>22</v>
@@ -15302,14 +15337,14 @@
       </c>
     </row>
     <row r="106" spans="1:45">
-      <c r="A106" s="20" t="s">
+      <c r="A106" t="s">
         <v>164</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C106">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D106" t="s">
         <v>22</v>
@@ -15387,14 +15422,14 @@
       </c>
     </row>
     <row r="107" spans="1:45">
-      <c r="A107" s="20" t="s">
+      <c r="A107" t="s">
         <v>164</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C107">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D107" t="s">
         <v>22</v>
@@ -15472,11 +15507,11 @@
       </c>
     </row>
     <row r="108" spans="1:45">
-      <c r="A108" s="20" t="s">
+      <c r="A108" t="s">
         <v>83</v>
       </c>
       <c r="C108">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D108" t="s">
         <v>22</v>
@@ -15532,11 +15567,11 @@
       </c>
     </row>
     <row r="109" spans="1:45">
-      <c r="A109" s="20" t="s">
+      <c r="A109" t="s">
         <v>83</v>
       </c>
       <c r="C109">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D109" t="s">
         <v>22</v>
@@ -15592,11 +15627,11 @@
       </c>
     </row>
     <row r="110" spans="1:45">
-      <c r="A110" s="20" t="s">
+      <c r="A110" t="s">
         <v>45</v>
       </c>
       <c r="C110">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D110" t="s">
         <v>22</v>
@@ -15655,11 +15690,11 @@
       </c>
     </row>
     <row r="111" spans="1:45">
-      <c r="A111" s="20" t="s">
+      <c r="A111" t="s">
         <v>45</v>
       </c>
       <c r="C111">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D111" t="s">
         <v>22</v>
@@ -15718,11 +15753,11 @@
       </c>
     </row>
     <row r="112" spans="1:45">
-      <c r="A112" s="20" t="s">
+      <c r="A112" t="s">
         <v>45</v>
       </c>
       <c r="C112">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D112" t="s">
         <v>22</v>
@@ -15781,14 +15816,14 @@
       </c>
     </row>
     <row r="113" spans="1:45">
-      <c r="A113" s="20" t="s">
+      <c r="A113" t="s">
         <v>202</v>
       </c>
       <c r="B113" t="s">
         <v>414</v>
       </c>
       <c r="C113">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D113" t="s">
         <v>22</v>
@@ -15859,14 +15894,14 @@
       </c>
     </row>
     <row r="114" spans="1:45">
-      <c r="A114" s="20" t="s">
+      <c r="A114" t="s">
         <v>202</v>
       </c>
       <c r="B114" t="s">
         <v>414</v>
       </c>
       <c r="C114">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D114" t="s">
         <v>22</v>
@@ -15937,14 +15972,14 @@
       </c>
     </row>
     <row r="115" spans="1:45">
-      <c r="A115" s="20" t="s">
+      <c r="A115" t="s">
         <v>92</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C115">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D115" t="s">
         <v>22</v>
@@ -16013,19 +16048,19 @@
         <f>IF(ISBLANK(I115), T115, SQRT(T115 ^ 2 / R115 + N115 ^ 2 / L115))</f>
         <v>0.97062585848815175</v>
       </c>
-      <c r="AC115" s="20" t="b">
+      <c r="AC115" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:45">
-      <c r="A116" s="20" t="s">
+      <c r="A116" t="s">
         <v>92</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C116">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D116" t="s">
         <v>22</v>
@@ -16094,19 +16129,19 @@
         <f>IF(ISBLANK(I116), T116, SQRT(T116 ^ 2 / R116 + N116 ^ 2 / L116))</f>
         <v>1.0628828966138939</v>
       </c>
-      <c r="AC116" s="20" t="b">
+      <c r="AC116" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:45">
-      <c r="A117" s="20" t="s">
+      <c r="A117" t="s">
         <v>92</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C117">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D117" t="s">
         <v>22</v>
@@ -16175,19 +16210,19 @@
         <f>IF(ISBLANK(I117), T117, SQRT(T117 ^ 2 / R117 + N117 ^ 2 / L117))</f>
         <v>0.97703141304754693</v>
       </c>
-      <c r="AC117" s="20" t="b">
+      <c r="AC117" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:45">
-      <c r="A118" s="20" t="s">
+      <c r="A118" t="s">
         <v>92</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C118">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D118" t="s">
         <v>22</v>
@@ -16256,19 +16291,19 @@
         <f>IF(ISBLANK(I118), T118, SQRT(T118 ^ 2 / R118 + N118 ^ 2 / L118))</f>
         <v>0.7154099868434618</v>
       </c>
-      <c r="AC118" s="20" t="b">
+      <c r="AC118" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:45">
-      <c r="A119" s="20" t="s">
+      <c r="A119" t="s">
         <v>92</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C119">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D119" t="s">
         <v>22</v>
@@ -16337,19 +16372,19 @@
         <f>IF(ISBLANK(I119), T119, SQRT(T119 ^ 2 / R119 + N119 ^ 2 / L119))</f>
         <v>0.78466582329708146</v>
       </c>
-      <c r="AC119" s="20" t="b">
+      <c r="AC119" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:45">
-      <c r="A120" s="20" t="s">
+      <c r="A120" t="s">
         <v>92</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C120">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D120" t="s">
         <v>22</v>
@@ -16418,7 +16453,7 @@
         <f>IF(ISBLANK(I120), T120, SQRT(T120 ^ 2 / R120 + N120 ^ 2 / L120))</f>
         <v>0.73662257154646438</v>
       </c>
-      <c r="AC120" s="20" t="b">
+      <c r="AC120" t="b">
         <v>1</v>
       </c>
       <c r="AJ120"/>
@@ -16429,14 +16464,14 @@
       <c r="AS120" s="2"/>
     </row>
     <row r="121" spans="1:45">
-      <c r="A121" s="20" t="s">
+      <c r="A121" t="s">
         <v>92</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C121">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D121" t="s">
         <v>22</v>
@@ -16505,7 +16540,7 @@
         <f>IF(ISBLANK(I121), T121, SQRT(T121 ^ 2 / R121 + N121 ^ 2 / L121))</f>
         <v>0.87591558722403673</v>
       </c>
-      <c r="AC121" s="20" t="b">
+      <c r="AC121" t="b">
         <v>1</v>
       </c>
       <c r="AJ121"/>
@@ -16516,14 +16551,14 @@
       <c r="AS121" s="2"/>
     </row>
     <row r="122" spans="1:45">
-      <c r="A122" s="20" t="s">
+      <c r="A122" t="s">
         <v>92</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C122">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D122" t="s">
         <v>22</v>
@@ -16592,19 +16627,19 @@
         <f>IF(ISBLANK(I122), T122, SQRT(T122 ^ 2 / R122 + N122 ^ 2 / L122))</f>
         <v>0.90080282408656309</v>
       </c>
-      <c r="AC122" s="20" t="b">
+      <c r="AC122" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:45">
-      <c r="A123" s="20" t="s">
+      <c r="A123" t="s">
         <v>92</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C123">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D123" t="s">
         <v>22</v>
@@ -16673,19 +16708,19 @@
         <f>IF(ISBLANK(I123), T123, SQRT(T123 ^ 2 / R123 + N123 ^ 2 / L123))</f>
         <v>0.90063526108951919</v>
       </c>
-      <c r="AC123" s="20" t="b">
+      <c r="AC123" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:45">
-      <c r="A124" s="20" t="s">
+      <c r="A124" t="s">
         <v>103</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>442</v>
       </c>
       <c r="C124">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D124" t="s">
         <v>22</v>
@@ -16738,11 +16773,14 @@
       </c>
     </row>
     <row r="125" spans="1:45">
-      <c r="A125" s="20" t="s">
+      <c r="A125" t="s">
         <v>69</v>
       </c>
+      <c r="B125" s="5" t="s">
+        <v>443</v>
+      </c>
       <c r="C125">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="D125" t="s">
         <v>22</v>
@@ -16754,7 +16792,7 @@
         <v>94</v>
       </c>
       <c r="G125" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -16798,11 +16836,14 @@
       </c>
     </row>
     <row r="126" spans="1:45">
-      <c r="A126" s="20" t="s">
+      <c r="A126" t="s">
         <v>69</v>
       </c>
+      <c r="B126" s="5" t="s">
+        <v>443</v>
+      </c>
       <c r="C126">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D126" t="s">
         <v>22</v>
@@ -16858,11 +16899,14 @@
       </c>
     </row>
     <row r="127" spans="1:45">
-      <c r="A127" s="20" t="s">
+      <c r="A127" t="s">
         <v>111</v>
       </c>
+      <c r="B127" s="5" t="s">
+        <v>445</v>
+      </c>
       <c r="C127">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="D127" t="s">
         <v>22</v>
@@ -16874,7 +16918,7 @@
         <v>94</v>
       </c>
       <c r="G127" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -16918,11 +16962,14 @@
       </c>
     </row>
     <row r="128" spans="1:45">
-      <c r="A128" s="20" t="s">
+      <c r="A128" t="s">
         <v>111</v>
       </c>
+      <c r="B128" s="5" t="s">
+        <v>445</v>
+      </c>
       <c r="C128">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="D128" t="s">
         <v>22</v>
@@ -16934,7 +16981,7 @@
         <v>94</v>
       </c>
       <c r="G128" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -16984,11 +17031,14 @@
       <c r="AS128" s="2"/>
     </row>
     <row r="129" spans="1:45">
-      <c r="A129" s="20" t="s">
+      <c r="A129" t="s">
         <v>71</v>
       </c>
+      <c r="B129" s="5" t="s">
+        <v>448</v>
+      </c>
       <c r="C129">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D129" t="s">
         <v>22</v>
@@ -17047,14 +17097,14 @@
       <c r="AS129" s="2"/>
     </row>
     <row r="130" spans="1:45">
-      <c r="A130" s="20" t="s">
+      <c r="A130" t="s">
         <v>196</v>
       </c>
       <c r="B130" t="s">
         <v>407</v>
       </c>
       <c r="C130">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D130" t="s">
         <v>22</v>
@@ -17116,14 +17166,14 @@
       <c r="AS130" s="2"/>
     </row>
     <row r="131" spans="1:45">
-      <c r="A131" s="20" t="s">
+      <c r="A131" t="s">
         <v>196</v>
       </c>
       <c r="B131" t="s">
         <v>407</v>
       </c>
       <c r="C131">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D131" t="s">
         <v>22</v>
@@ -17185,26 +17235,26 @@
       <c r="AQ131"/>
     </row>
     <row r="132" spans="1:45">
-      <c r="A132" s="20" t="s">
+      <c r="A132" t="s">
         <v>164</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C132">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D132" t="s">
         <v>22</v>
       </c>
       <c r="E132" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F132" t="s">
         <v>94</v>
       </c>
       <c r="G132" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="H132">
         <v>9</v>
@@ -17273,26 +17323,26 @@
       <c r="AQ132"/>
     </row>
     <row r="133" spans="1:45">
-      <c r="A133" s="20" t="s">
+      <c r="A133" t="s">
         <v>164</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C133">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D133" t="s">
         <v>22</v>
       </c>
       <c r="E133" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F133" t="s">
         <v>94</v>
       </c>
       <c r="G133" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="H133">
         <v>15</v>
@@ -17361,26 +17411,26 @@
       <c r="AQ133"/>
     </row>
     <row r="134" spans="1:45">
-      <c r="A134" s="20" t="s">
+      <c r="A134" t="s">
         <v>164</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C134">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D134" t="s">
         <v>22</v>
       </c>
       <c r="E134" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F134" t="s">
         <v>94</v>
       </c>
       <c r="G134" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="H134">
         <v>21</v>
@@ -17449,26 +17499,26 @@
       <c r="AQ134"/>
     </row>
     <row r="135" spans="1:45">
-      <c r="A135" s="20" t="s">
+      <c r="A135" t="s">
         <v>164</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C135">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D135" t="s">
         <v>22</v>
       </c>
       <c r="E135" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F135" t="s">
         <v>94</v>
       </c>
       <c r="G135" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="H135">
         <v>9</v>
@@ -17537,26 +17587,26 @@
       <c r="AQ135"/>
     </row>
     <row r="136" spans="1:45">
-      <c r="A136" s="20" t="s">
+      <c r="A136" t="s">
         <v>164</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C136">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D136" t="s">
         <v>22</v>
       </c>
       <c r="E136" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F136" t="s">
         <v>94</v>
       </c>
       <c r="G136" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="H136">
         <v>15</v>
@@ -17625,26 +17675,26 @@
       <c r="AQ136"/>
     </row>
     <row r="137" spans="1:45">
-      <c r="A137" s="20" t="s">
+      <c r="A137" t="s">
         <v>164</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>432</v>
       </c>
       <c r="C137">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D137" t="s">
         <v>22</v>
       </c>
       <c r="E137" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F137" t="s">
         <v>94</v>
       </c>
       <c r="G137" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="H137">
         <v>21</v>
@@ -17713,14 +17763,14 @@
       <c r="AQ137"/>
     </row>
     <row r="138" spans="1:45">
-      <c r="A138" s="20" t="s">
+      <c r="A138" t="s">
         <v>202</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="5" t="s">
         <v>414</v>
       </c>
       <c r="C138">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D138" t="s">
         <v>22</v>
@@ -17794,14 +17844,14 @@
       <c r="AQ138"/>
     </row>
     <row r="139" spans="1:45">
-      <c r="A139" s="20" t="s">
+      <c r="A139" t="s">
         <v>202</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="5" t="s">
         <v>414</v>
       </c>
       <c r="C139">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D139" t="s">
         <v>22</v>
@@ -17875,14 +17925,14 @@
       <c r="AQ139"/>
     </row>
     <row r="140" spans="1:45">
-      <c r="A140" s="20" t="s">
+      <c r="A140" t="s">
         <v>200</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="5" t="s">
         <v>412</v>
       </c>
       <c r="C140">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D140" t="s">
         <v>22</v>
@@ -17989,6 +18039,14 @@
     <hyperlink ref="B105" r:id="rId47" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{5AEDDA62-72BA-4AE4-9835-3C9035C844D0}"/>
     <hyperlink ref="B106" r:id="rId48" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{20D34FE8-4A35-4191-B36A-539946CE2F02}"/>
     <hyperlink ref="B107" r:id="rId49" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{06D257CE-F3A1-4BC5-A089-5CC8C400DFFB}"/>
+    <hyperlink ref="B125" r:id="rId50" xr:uid="{5CD56F0A-D88F-4B69-9BFD-24E6DE7673EB}"/>
+    <hyperlink ref="B126" r:id="rId51" xr:uid="{68180BF0-D74B-47AB-8548-69AD4EA4AFD5}"/>
+    <hyperlink ref="B127" r:id="rId52" xr:uid="{166012F6-ECEC-4E51-B9B6-2CDD64D45AC3}"/>
+    <hyperlink ref="B128" r:id="rId53" xr:uid="{4341EF26-B858-481F-A28F-CC4E96AD2855}"/>
+    <hyperlink ref="B129" r:id="rId54" xr:uid="{41DD919E-5396-4600-AA09-0F92B0A0B9C1}"/>
+    <hyperlink ref="B138" r:id="rId55" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=7yiFtW&amp;cid=68fb9a55%2Db8f3%2D4c55%2Dae2a%2Df5cc58a16d15&amp;FolderCTID=0x012000C93EC9BF0A69C541B8FA2022D55A7013&amp;isAscending=false&amp;sortField=Modified&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FSong%202022%20Effects%20of%20Maternal%20Adjustment%20Enhancement%20Program%20Using%20Mobile%2DBased%20Education%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;q=Song&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS&amp;parentview=7" xr:uid="{AFEB6DBE-8080-42EB-A8ED-773E27C875E6}"/>
+    <hyperlink ref="B139" r:id="rId56" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=7yiFtW&amp;cid=68fb9a55%2Db8f3%2D4c55%2Dae2a%2Df5cc58a16d15&amp;FolderCTID=0x012000C93EC9BF0A69C541B8FA2022D55A7013&amp;isAscending=false&amp;sortField=Modified&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FSong%202022%20Effects%20of%20Maternal%20Adjustment%20Enhancement%20Program%20Using%20Mobile%2DBased%20Education%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;q=Song&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS&amp;parentview=7" xr:uid="{049DA949-9BFC-4AD1-A955-81BAB32CCDFE}"/>
+    <hyperlink ref="B140" r:id="rId57" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=7yiFtW&amp;cid=68fb9a55%2Db8f3%2D4c55%2Dae2a%2Df5cc58a16d15&amp;FolderCTID=0x012000C93EC9BF0A69C541B8FA2022D55A7013&amp;isAscending=false&amp;sortField=Modified&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FZuckerman%202022%20Small%20moments%2C%20big%20impact%20Pilot%20trial%20of%20a%20relational%20health%20app%20for%20primary%20care%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;q=Small%20Moments%2C%20Big%20Impact&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS&amp;parentview=7" xr:uid="{4462B5E2-D370-455C-989A-5FD63A558474}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18012,82 +18070,82 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="18" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="G1" s="19" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="10"/>
       <c r="M1" s="19" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="N1" s="19"/>
       <c r="Q1" s="19" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
       <c r="U1" s="18" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="V1" s="18"/>
       <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="K2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -19033,15 +19091,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CBCD076DB4944242BD8F10DB27929B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="76d6280827467d84939e4694bc88b638">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f1c3b6d-7f32-4752-9b60-8760effeb2ab" xmlns:ns3="b77b1af8-43ce-437e-80a0-2a6bb447a677" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74c914b0449d12a5aaf279a9afdd045c" ns2:_="" ns3:_="">
     <xsd:import namespace="6f1c3b6d-7f32-4752-9b60-8760effeb2ab"/>
@@ -19272,6 +19321,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -19284,11 +19342,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C637C4C-9A48-4ADA-A1DE-A69ED46A1145}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBE96651-E477-4C50-BC89-C335725EFCB2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBE96651-E477-4C50-BC89-C335725EFCB2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C637C4C-9A48-4ADA-A1DE-A69ED46A1145}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Fix typo in study name; Add study summaries table to results
</commit_message>
<xml_diff>
--- a/data/data_extraction_te_20230205.xlsx
+++ b/data/data_extraction_te_20230205.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\times\Repos\opie-2023-online-parenting-meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74B658B9-6C3D-4AF0-ADF0-1DCA8E2523AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3F5B26-7040-4051-819E-8D388AE98907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,8 @@
     <sheet name="Removed Studies (2 ints)" sheetId="8" r:id="rId5"/>
     <sheet name="Studies to Check" sheetId="2" r:id="rId6"/>
     <sheet name="Study Statistics" sheetId="4" r:id="rId7"/>
-    <sheet name="Calculators" sheetId="6" r:id="rId8"/>
+    <sheet name="Delivery Mode Comp" sheetId="9" r:id="rId8"/>
+    <sheet name="Calculators" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,8 +58,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={91C9DF83-59D8-4DA1-BA3E-0B5C816AEF8E}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{91C9DF83-59D8-4DA1-BA3E-0B5C816AEF8E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    @Felicity Painter these are our final studies</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2270" uniqueCount="466">
   <si>
     <t>study</t>
   </si>
@@ -1639,7 +1658,7 @@
     <numFmt numFmtId="164" formatCode="0.00000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1662,6 +1681,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1712,7 +1737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1741,8 +1766,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2074,6 +2097,17 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2023-04-04T23:12:47.06" personId="{01FBE822-907B-4C9D-9E9E-52ED858BD6FA}" id="{91C9DF83-59D8-4DA1-BA3E-0B5C816AEF8E}">
+    <text>@Felicity Painter these are our final studies</text>
+    <mentions>
+      <mention mentionpersonId="{0B4DB856-515E-4CE8-9E53-7BD9ADEBBC6C}" mentionId="{EC6CBFA3-0448-4CB6-ABB3-F48A1C97A840}" startIndex="0" length="17"/>
+    </mentions>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U65"/>
@@ -7684,9 +7718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{035708AA-504B-40B6-A564-C20BC08724FD}">
   <dimension ref="A1:AS140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P138" sqref="P138"/>
+      <selection pane="topRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9652,7 +9686,7 @@
         <f t="shared" si="3"/>
         <v>1.060525476221239</v>
       </c>
-      <c r="AC25" s="18" t="b">
+      <c r="AC25" t="b">
         <v>1</v>
       </c>
       <c r="AJ25"/>
@@ -9721,7 +9755,7 @@
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
-      <c r="AC26" s="19" t="b">
+      <c r="AC26" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9784,7 +9818,7 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
-      <c r="AC27" s="19" t="b">
+      <c r="AC27" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9866,7 +9900,7 @@
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
       <c r="AB28" s="3"/>
-      <c r="AC28" s="19" t="b">
+      <c r="AC28" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9948,7 +9982,7 @@
       <c r="Z29" s="3"/>
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
-      <c r="AC29" s="19" t="b">
+      <c r="AC29" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10030,7 +10064,7 @@
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
-      <c r="AC30" s="19" t="b">
+      <c r="AC30" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10093,7 +10127,7 @@
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
-      <c r="AC31" s="19" t="b">
+      <c r="AC31" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10156,7 +10190,7 @@
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
-      <c r="AC32" s="19" t="b">
+      <c r="AC32" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10219,7 +10253,7 @@
       <c r="Z33">
         <v>2.082957196018731E-2</v>
       </c>
-      <c r="AC33" s="18" t="b">
+      <c r="AC33" t="b">
         <v>1</v>
       </c>
       <c r="AJ33"/>
@@ -11317,7 +11351,7 @@
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>403</v>
@@ -11386,7 +11420,7 @@
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>403</v>
@@ -11704,7 +11738,7 @@
       <c r="Z54" s="3"/>
       <c r="AA54" s="3"/>
       <c r="AB54" s="3"/>
-      <c r="AC54" s="19" t="b">
+      <c r="AC54" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -11767,7 +11801,7 @@
       <c r="Z55" s="3"/>
       <c r="AA55" s="3"/>
       <c r="AB55" s="3"/>
-      <c r="AC55" s="19" t="b">
+      <c r="AC55" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -11825,7 +11859,7 @@
         <f t="shared" si="7"/>
         <v>13.3</v>
       </c>
-      <c r="AC56" s="19" t="b">
+      <c r="AC56" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -11888,7 +11922,7 @@
       <c r="AB57">
         <v>0.18112244897959184</v>
       </c>
-      <c r="AC57" s="19" t="b">
+      <c r="AC57" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -11951,7 +11985,7 @@
       <c r="AB58">
         <v>0.17602040816326531</v>
       </c>
-      <c r="AC58" s="19" t="b">
+      <c r="AC58" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12014,7 +12048,7 @@
       <c r="AB59">
         <v>0.19642857142857142</v>
       </c>
-      <c r="AC59" s="19" t="b">
+      <c r="AC59" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12072,7 +12106,7 @@
         <f t="shared" si="7"/>
         <v>10.62</v>
       </c>
-      <c r="AC60" s="18" t="b">
+      <c r="AC60" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12130,7 +12164,7 @@
         <f t="shared" si="7"/>
         <v>12.24</v>
       </c>
-      <c r="AC61" s="18" t="b">
+      <c r="AC61" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12188,7 +12222,7 @@
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="AC62" s="18" t="b">
+      <c r="AC62" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12269,7 +12303,7 @@
         <f t="shared" si="7"/>
         <v>1.0526259496902923</v>
       </c>
-      <c r="AC63" s="18" t="b">
+      <c r="AC63" t="b">
         <v>1</v>
       </c>
       <c r="AJ63"/>
@@ -12356,7 +12390,7 @@
         <f t="shared" si="7"/>
         <v>1.0718475371325638</v>
       </c>
-      <c r="AC64" s="18" t="b">
+      <c r="AC64" t="b">
         <v>1</v>
       </c>
       <c r="AJ64"/>
@@ -12420,7 +12454,7 @@
         <f t="shared" si="7"/>
         <v>7.52</v>
       </c>
-      <c r="AC65" s="19" t="b">
+      <c r="AC65" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12478,7 +12512,7 @@
         <f t="shared" ref="X66:X92" si="11">IF(ISBLANK(I66), T66, SQRT(T66 ^ 2 / R66 + N66 ^ 2 / L66))</f>
         <v>7.1</v>
       </c>
-      <c r="AC66" s="19" t="b">
+      <c r="AC66" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12556,7 +12590,7 @@
         <f t="shared" si="11"/>
         <v>2.0422767895890406</v>
       </c>
-      <c r="AC67" s="19" t="b">
+      <c r="AC67" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12634,7 +12668,7 @@
         <f t="shared" si="11"/>
         <v>2.1760273210510901</v>
       </c>
-      <c r="AC68" s="19" t="b">
+      <c r="AC68" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12712,7 +12746,7 @@
         <f t="shared" si="11"/>
         <v>2.2781413296443662</v>
       </c>
-      <c r="AC69" s="19" t="b">
+      <c r="AC69" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12770,7 +12804,7 @@
         <f t="shared" si="11"/>
         <v>3.03</v>
       </c>
-      <c r="AC70" s="19" t="b">
+      <c r="AC70" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -12828,7 +12862,7 @@
         <f t="shared" si="11"/>
         <v>7.81</v>
       </c>
-      <c r="AC71" s="18" t="b">
+      <c r="AC71" t="b">
         <v>0</v>
       </c>
     </row>
@@ -12886,7 +12920,7 @@
         <f t="shared" si="11"/>
         <v>8.4</v>
       </c>
-      <c r="AC72" s="18" t="b">
+      <c r="AC72" t="b">
         <v>0</v>
       </c>
     </row>
@@ -12944,7 +12978,7 @@
         <f t="shared" si="11"/>
         <v>21.9</v>
       </c>
-      <c r="AC73" s="19" t="b">
+      <c r="AC73" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -13007,7 +13041,7 @@
       <c r="AB74">
         <v>0.23469387799999999</v>
       </c>
-      <c r="AC74" s="19" t="b">
+      <c r="AC74" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -13070,7 +13104,7 @@
       <c r="AB75">
         <v>0.216836735</v>
       </c>
-      <c r="AC75" s="19" t="b">
+      <c r="AC75" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14451,7 +14485,7 @@
       <c r="Z94">
         <v>0.16600000000000001</v>
       </c>
-      <c r="AC94" s="18" t="b">
+      <c r="AC94" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14532,7 +14566,7 @@
         <f t="shared" si="13"/>
         <v>0.20650932275832098</v>
       </c>
-      <c r="AC95" s="18" t="b">
+      <c r="AC95" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14613,7 +14647,7 @@
         <f t="shared" si="13"/>
         <v>0.23597215332080423</v>
       </c>
-      <c r="AC96" s="18" t="b">
+      <c r="AC96" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14671,7 +14705,7 @@
         <f t="shared" si="13"/>
         <v>2.92</v>
       </c>
-      <c r="AC97" s="19" t="b">
+      <c r="AC97" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14728,7 +14762,7 @@
         <f t="shared" si="13"/>
         <v>3.13</v>
       </c>
-      <c r="AC98" s="19" t="b">
+      <c r="AC98" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14806,7 +14840,7 @@
         <f t="shared" si="13"/>
         <v>3.0048130508549504</v>
       </c>
-      <c r="AC99" s="19" t="b">
+      <c r="AC99" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14884,7 +14918,7 @@
         <f t="shared" si="13"/>
         <v>2.9884750521386159</v>
       </c>
-      <c r="AC100" s="19" t="b">
+      <c r="AC100" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14962,7 +14996,7 @@
         <f t="shared" si="13"/>
         <v>3.1940334197470839</v>
       </c>
-      <c r="AC101" s="19" t="b">
+      <c r="AC101" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15035,7 +15069,7 @@
       <c r="Z102" s="3"/>
       <c r="AA102" s="3"/>
       <c r="AB102" s="3"/>
-      <c r="AC102" s="19" t="b">
+      <c r="AC102" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15108,7 +15142,7 @@
       <c r="Z103" s="3"/>
       <c r="AA103" s="3"/>
       <c r="AB103" s="3"/>
-      <c r="AC103" s="19" t="b">
+      <c r="AC103" s="3" t="b">
         <v>1</v>
       </c>
       <c r="AJ103"/>
@@ -15187,7 +15221,7 @@
       <c r="Z104" s="3"/>
       <c r="AA104" s="3"/>
       <c r="AB104" s="3"/>
-      <c r="AC104" s="19" t="b">
+      <c r="AC104" s="3" t="b">
         <v>1</v>
       </c>
       <c r="AJ104"/>
@@ -15266,7 +15300,7 @@
       <c r="Z105" s="3"/>
       <c r="AA105" s="3"/>
       <c r="AB105" s="3"/>
-      <c r="AC105" s="19" t="b">
+      <c r="AC105" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15339,7 +15373,7 @@
       <c r="Z106" s="3"/>
       <c r="AA106" s="3"/>
       <c r="AB106" s="3"/>
-      <c r="AC106" s="19" t="b">
+      <c r="AC106" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15412,7 +15446,7 @@
       <c r="Z107" s="3"/>
       <c r="AA107" s="3"/>
       <c r="AB107" s="3"/>
-      <c r="AC107" s="19" t="b">
+      <c r="AC107" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15472,7 +15506,7 @@
         <f t="shared" si="13"/>
         <v>22.3</v>
       </c>
-      <c r="AC108" s="19" t="b">
+      <c r="AC108" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15532,7 +15566,7 @@
         <f t="shared" si="13"/>
         <v>22.5</v>
       </c>
-      <c r="AC109" s="19" t="b">
+      <c r="AC109" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -15595,7 +15629,7 @@
       <c r="AB110">
         <v>0.14540816300000001</v>
       </c>
-      <c r="AC110" s="19" t="b">
+      <c r="AC110" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16618,7 +16652,7 @@
         <f t="shared" si="13"/>
         <v>0.90063526108951919</v>
       </c>
-      <c r="AC123" s="18" t="b">
+      <c r="AC123" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16678,7 +16712,7 @@
         <f t="shared" si="13"/>
         <v>17.670000000000002</v>
       </c>
-      <c r="AC124" s="18" t="b">
+      <c r="AC124" t="b">
         <v>0</v>
       </c>
     </row>
@@ -16741,7 +16775,7 @@
         <f t="shared" si="13"/>
         <v>12.45</v>
       </c>
-      <c r="AC125" s="19" t="b">
+      <c r="AC125" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16804,7 +16838,7 @@
         <f t="shared" si="13"/>
         <v>4.84</v>
       </c>
-      <c r="AC126" s="19" t="b">
+      <c r="AC126" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16867,7 +16901,7 @@
         <f t="shared" si="13"/>
         <v>11.34</v>
       </c>
-      <c r="AC127" s="19" t="b">
+      <c r="AC127" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -16930,7 +16964,7 @@
         <f t="shared" si="13"/>
         <v>12.92</v>
       </c>
-      <c r="AC128" s="19" t="b">
+      <c r="AC128" s="3" t="b">
         <v>1</v>
       </c>
       <c r="AJ128"/>
@@ -16996,7 +17030,7 @@
         <f t="shared" si="13"/>
         <v>5.98</v>
       </c>
-      <c r="AC129" s="19" t="b">
+      <c r="AC129" s="3" t="b">
         <v>1</v>
       </c>
       <c r="AJ129"/>
@@ -17065,7 +17099,7 @@
       <c r="Z130">
         <v>2.0914805120809073E-2</v>
       </c>
-      <c r="AC130" s="18" t="b">
+      <c r="AC130" t="b">
         <v>1</v>
       </c>
       <c r="AJ130"/>
@@ -17134,7 +17168,7 @@
       <c r="Z131">
         <v>2.6226970119784712E-2</v>
       </c>
-      <c r="AC131" s="18" t="b">
+      <c r="AC131" t="b">
         <v>1</v>
       </c>
       <c r="AF131" s="2"/>
@@ -17875,6 +17909,2238 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBEEAEB-E98C-4248-AAC1-ACAFA775285F}">
+  <dimension ref="A1:AS39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AQ1" s="9"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>68</v>
+      </c>
+      <c r="J2" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="K2">
+        <v>3.8</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="O2">
+        <v>64</v>
+      </c>
+      <c r="P2">
+        <v>3.39</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>7.68</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2">
+        <f t="shared" ref="U2:U4" si="0">P2-J2</f>
+        <v>-1.81</v>
+      </c>
+      <c r="V2">
+        <f t="shared" ref="V2:V4" si="1">IF(ISBLANK(I2), Q2, SQRT(Q2 ^ 2 / O2 + K2 ^ 2 / I2))</f>
+        <v>1.0648722651926241</v>
+      </c>
+      <c r="W2">
+        <f t="shared" ref="W2:W4" si="2">S2 - M2</f>
+        <v>0</v>
+      </c>
+      <c r="X2" t="e">
+        <f t="shared" ref="X2:X4" si="3">IF(ISBLANK(I2), T2, SQRT(T2 ^ 2 / R2 + N2 ^ 2 / L2))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AQ2" s="2"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" s="4">
+        <v>68</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="K3">
+        <v>3.8</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="O3">
+        <v>56</v>
+      </c>
+      <c r="P3">
+        <v>1.91</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>6.62</v>
+      </c>
+      <c r="T3" s="3"/>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>-3.29</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="1"/>
+        <v>0.99746253694313847</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AQ3" s="2"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4" s="4">
+        <v>68</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="K4">
+        <v>3.8</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="O4">
+        <v>61</v>
+      </c>
+      <c r="P4">
+        <v>3.4</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>6.94</v>
+      </c>
+      <c r="T4" s="3"/>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>-1.8000000000000003</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="1"/>
+        <v>1.000959616713494</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="X4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AQ4" s="2"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>68</v>
+      </c>
+      <c r="J6" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="K6">
+        <v>4.5</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="O6">
+        <v>64</v>
+      </c>
+      <c r="P6">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>9.94</v>
+      </c>
+      <c r="T6" s="3"/>
+      <c r="U6">
+        <f t="shared" ref="U6:U8" si="4">P6-J6</f>
+        <v>-2.67</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V8" si="5">IF(ISBLANK(I6), Q6, SQRT(Q6 ^ 2 / O6 + K6 ^ 2 / I6))</f>
+        <v>1.3570557717526051</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ref="W6:W8" si="6">S6 - M6</f>
+        <v>0</v>
+      </c>
+      <c r="X6" t="e">
+        <f t="shared" ref="X6:X8" si="7">IF(ISBLANK(I6), T6, SQRT(T6 ^ 2 / R6 + N6 ^ 2 / L6))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AQ6" s="2"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C7">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>68</v>
+      </c>
+      <c r="J7" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="K7">
+        <v>4.5</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="O7">
+        <v>56</v>
+      </c>
+      <c r="P7">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>9.01</v>
+      </c>
+      <c r="T7" s="3"/>
+      <c r="U7">
+        <f t="shared" si="4"/>
+        <v>-4.8900000000000006</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="5"/>
+        <v>1.3219072435326926</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AQ7" s="2"/>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="4">
+        <v>68</v>
+      </c>
+      <c r="J8" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="K8">
+        <v>4.5</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="O8">
+        <v>61</v>
+      </c>
+      <c r="P8">
+        <v>4.34</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>10.71</v>
+      </c>
+      <c r="T8" s="3"/>
+      <c r="U8">
+        <f t="shared" si="4"/>
+        <v>-3.0600000000000005</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="5"/>
+        <v>1.4758689642425145</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AQ8" s="2"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C10">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>68</v>
+      </c>
+      <c r="J10">
+        <v>45.7</v>
+      </c>
+      <c r="K10">
+        <v>6.9</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="O10">
+        <v>64</v>
+      </c>
+      <c r="P10">
+        <v>52.44</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>14.08</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ref="U10:U12" si="8">P10-J10</f>
+        <v>6.7399999999999949</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ref="V10:V12" si="9">IF(ISBLANK(I10), Q10, SQRT(Q10 ^ 2 / O10 + K10 ^ 2 / I10))</f>
+        <v>1.948780916066126</v>
+      </c>
+      <c r="W10">
+        <f t="shared" ref="W10:W12" si="10">S10 - M10</f>
+        <v>0</v>
+      </c>
+      <c r="X10" t="e">
+        <f t="shared" ref="X10:X12" si="11">IF(ISBLANK(I10), T10, SQRT(T10 ^ 2 / R10 + N10 ^ 2 / L10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AQ10" s="2"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C11">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="4">
+        <v>68</v>
+      </c>
+      <c r="J11">
+        <v>45.7</v>
+      </c>
+      <c r="K11">
+        <v>6.9</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="O11">
+        <v>56</v>
+      </c>
+      <c r="P11">
+        <v>57.9</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>14.47</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="8"/>
+        <v>12.199999999999996</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="9"/>
+        <v>2.1069152098935238</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X11" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AQ11" s="2"/>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C12">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12" s="4">
+        <v>68</v>
+      </c>
+      <c r="J12">
+        <v>45.7</v>
+      </c>
+      <c r="K12">
+        <v>6.9</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="O12">
+        <v>61</v>
+      </c>
+      <c r="P12">
+        <v>60.72</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>15.56</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="8"/>
+        <v>15.019999999999996</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="9"/>
+        <v>2.1608383717112201</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X12" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC12" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AQ12" s="2"/>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C14">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>68</v>
+      </c>
+      <c r="J14">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="K14">
+        <v>11.7</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="O14">
+        <v>64</v>
+      </c>
+      <c r="P14">
+        <v>82.92</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>20.82</v>
+      </c>
+      <c r="U14">
+        <f t="shared" ref="U14:U16" si="12">P14-J14</f>
+        <v>3.519999999999996</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ref="V14:V16" si="13">IF(ISBLANK(I14), Q14, SQRT(Q14 ^ 2 / O14 + K14 ^ 2 / I14))</f>
+        <v>2.9641346941888651</v>
+      </c>
+      <c r="W14">
+        <f t="shared" ref="W14:W16" si="14">S14 - M14</f>
+        <v>0</v>
+      </c>
+      <c r="X14" t="e">
+        <f t="shared" ref="X14:X16" si="15">IF(ISBLANK(I14), T14, SQRT(T14 ^ 2 / R14 + N14 ^ 2 / L14))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC14" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AQ14" s="2"/>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C15">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" t="s">
+        <v>160</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15" s="4">
+        <v>68</v>
+      </c>
+      <c r="J15">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="K15">
+        <v>11.7</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="O15">
+        <v>56</v>
+      </c>
+      <c r="P15">
+        <v>85.98</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="12"/>
+        <v>6.5799999999999983</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="13"/>
+        <v>2.9658564204496964</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="X15" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AQ15" s="2"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16" s="4">
+        <v>68</v>
+      </c>
+      <c r="J16">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="K16">
+        <v>11.7</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="O16">
+        <v>61</v>
+      </c>
+      <c r="P16">
+        <v>85.86</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>21.78</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="12"/>
+        <v>6.4599999999999937</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="13"/>
+        <v>3.1288367459544935</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="X16" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC16" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AQ16" s="2"/>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
+        <v>416</v>
+      </c>
+      <c r="C18">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="O18">
+        <v>233</v>
+      </c>
+      <c r="P18">
+        <v>41.79</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0.30528675044947495</v>
+      </c>
+      <c r="R18" s="4">
+        <v>250</v>
+      </c>
+      <c r="S18" s="3">
+        <v>41.83</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="U18">
+        <f t="shared" ref="U18:U20" si="16">P18-J18</f>
+        <v>41.79</v>
+      </c>
+      <c r="V18">
+        <f t="shared" ref="V18:V20" si="17">IF(ISBLANK(I18), Q18, SQRT(Q18 ^ 2 / O18 + K18 ^ 2 / I18))</f>
+        <v>0.30528675044947495</v>
+      </c>
+      <c r="W18">
+        <f t="shared" ref="W18:W20" si="18">S18 - M18</f>
+        <v>41.83</v>
+      </c>
+      <c r="X18">
+        <f t="shared" ref="X18:X20" si="19">IF(ISBLANK(I18), T18, SQRT(T18 ^ 2 / R18 + N18 ^ 2 / L18))</f>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="AC18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AS18" s="2"/>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
+        <v>416</v>
+      </c>
+      <c r="C19">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F19" t="s">
+        <v>180</v>
+      </c>
+      <c r="H19">
+        <v>15</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="O19">
+        <v>231</v>
+      </c>
+      <c r="P19">
+        <v>41.83</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0.30397368307141326</v>
+      </c>
+      <c r="R19" s="4">
+        <v>247</v>
+      </c>
+      <c r="S19" s="3">
+        <v>41.8</v>
+      </c>
+      <c r="T19" s="3">
+        <v>0.31432467291003424</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="16"/>
+        <v>41.83</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="17"/>
+        <v>0.30397368307141326</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="18"/>
+        <v>41.8</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="19"/>
+        <v>0.31432467291003424</v>
+      </c>
+      <c r="AC19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
+      <c r="AS19" s="2"/>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C20">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" t="s">
+        <v>180</v>
+      </c>
+      <c r="H20">
+        <v>21</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="O20">
+        <v>216</v>
+      </c>
+      <c r="P20">
+        <v>42.07</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0.29393876913398137</v>
+      </c>
+      <c r="R20" s="4">
+        <v>240</v>
+      </c>
+      <c r="S20" s="3">
+        <v>42.22</v>
+      </c>
+      <c r="T20" s="3">
+        <v>0.30983866769659335</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="16"/>
+        <v>42.07</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="17"/>
+        <v>0.29393876913398137</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="18"/>
+        <v>42.22</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="19"/>
+        <v>0.30983866769659335</v>
+      </c>
+      <c r="AC20" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
+      <c r="AS20" s="2"/>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C22">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" t="s">
+        <v>433</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22">
+        <v>233</v>
+      </c>
+      <c r="P22">
+        <v>75.11</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1.2211470019999999</v>
+      </c>
+      <c r="R22">
+        <v>250</v>
+      </c>
+      <c r="S22">
+        <v>76.040000000000006</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1.423024947</v>
+      </c>
+      <c r="U22">
+        <f t="shared" ref="U22:U27" si="20">P22-J22</f>
+        <v>75.11</v>
+      </c>
+      <c r="V22">
+        <f t="shared" ref="V22:V27" si="21">IF(ISBLANK(I22), Q22, SQRT(Q22 ^ 2 / O22 + K22 ^ 2 / I22))</f>
+        <v>1.2211470019999999</v>
+      </c>
+      <c r="W22">
+        <f t="shared" ref="W22:W27" si="22">S22 - M22</f>
+        <v>76.040000000000006</v>
+      </c>
+      <c r="X22">
+        <f t="shared" ref="X22:X27" si="23">IF(ISBLANK(I22), T22, SQRT(T22 ^ 2 / R22 + N22 ^ 2 / L22))</f>
+        <v>1.423024947</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AQ22" s="2"/>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C23">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" t="s">
+        <v>433</v>
+      </c>
+      <c r="H23">
+        <v>15</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23">
+        <v>231</v>
+      </c>
+      <c r="P23">
+        <v>75.61</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1.215894732</v>
+      </c>
+      <c r="R23">
+        <v>247</v>
+      </c>
+      <c r="S23">
+        <v>75.56</v>
+      </c>
+      <c r="T23" s="3">
+        <v>1.4144610280000001</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="20"/>
+        <v>75.61</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="21"/>
+        <v>1.215894732</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="22"/>
+        <v>75.56</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="23"/>
+        <v>1.4144610280000001</v>
+      </c>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AS23" s="2"/>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C24">
+        <v>103</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" t="s">
+        <v>433</v>
+      </c>
+      <c r="H24">
+        <v>21</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24">
+        <v>216</v>
+      </c>
+      <c r="P24">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>1.175755077</v>
+      </c>
+      <c r="R24">
+        <v>240</v>
+      </c>
+      <c r="S24">
+        <v>76.3</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1.394274005</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="20"/>
+        <v>75.650000000000006</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="21"/>
+        <v>1.175755077</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="22"/>
+        <v>76.3</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="23"/>
+        <v>1.394274005</v>
+      </c>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AS24" s="2"/>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C25">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" t="s">
+        <v>434</v>
+      </c>
+      <c r="H25">
+        <v>9</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25">
+        <v>233</v>
+      </c>
+      <c r="P25">
+        <v>38.96</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="R25">
+        <v>250</v>
+      </c>
+      <c r="S25">
+        <v>39.43</v>
+      </c>
+      <c r="T25" s="3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="20"/>
+        <v>38.96</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="21"/>
+        <v>1.07</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="22"/>
+        <v>39.43</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="23"/>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AQ25" s="2"/>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C26">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" t="s">
+        <v>434</v>
+      </c>
+      <c r="H26">
+        <v>15</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26">
+        <v>231</v>
+      </c>
+      <c r="P26">
+        <v>38.840000000000003</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="R26">
+        <v>247</v>
+      </c>
+      <c r="S26">
+        <v>38.64</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="20"/>
+        <v>38.840000000000003</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="21"/>
+        <v>1.06</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="22"/>
+        <v>38.64</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="23"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AQ26" s="2"/>
+    </row>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C27">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" t="s">
+        <v>434</v>
+      </c>
+      <c r="H27">
+        <v>21</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27">
+        <v>216</v>
+      </c>
+      <c r="P27">
+        <v>38.549999999999997</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="R27">
+        <v>240</v>
+      </c>
+      <c r="S27">
+        <v>39.28</v>
+      </c>
+      <c r="T27" s="3">
+        <v>1.08</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="20"/>
+        <v>38.549999999999997</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="21"/>
+        <v>1.03</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="22"/>
+        <v>39.28</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="23"/>
+        <v>1.08</v>
+      </c>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="2"/>
+      <c r="AK27" s="2"/>
+      <c r="AQ27" s="2"/>
+    </row>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29">
+        <v>131</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>449</v>
+      </c>
+      <c r="F29" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" t="s">
+        <v>450</v>
+      </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="L29" s="4"/>
+      <c r="O29">
+        <v>233</v>
+      </c>
+      <c r="P29">
+        <v>20.82</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0.61057350099999996</v>
+      </c>
+      <c r="R29" s="4">
+        <v>250</v>
+      </c>
+      <c r="S29" s="3">
+        <v>20.59</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0.63245553200000004</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29:U34" si="24">P29-J29</f>
+        <v>20.82</v>
+      </c>
+      <c r="V29">
+        <f t="shared" ref="V29:V34" si="25">IF(ISBLANK(I29), Q29, SQRT(Q29 ^ 2 / O29 + K29 ^ 2 / I29))</f>
+        <v>0.61057350099999996</v>
+      </c>
+      <c r="W29">
+        <f t="shared" ref="W29:W34" si="26">S29 - M29</f>
+        <v>20.59</v>
+      </c>
+      <c r="X29">
+        <f t="shared" ref="X29:X34" si="27">IF(ISBLANK(I29), T29, SQRT(T29 ^ 2 / R29 + N29 ^ 2 / L29))</f>
+        <v>0.63245553200000004</v>
+      </c>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C30">
+        <v>132</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>449</v>
+      </c>
+      <c r="F30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" t="s">
+        <v>450</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="3"/>
+      <c r="L30" s="4"/>
+      <c r="O30">
+        <v>231</v>
+      </c>
+      <c r="P30">
+        <v>20.22</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0.60794736599999999</v>
+      </c>
+      <c r="R30" s="4">
+        <v>247</v>
+      </c>
+      <c r="S30" s="3">
+        <v>20.21</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0.628649346</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="24"/>
+        <v>20.22</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="25"/>
+        <v>0.60794736599999999</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="26"/>
+        <v>20.21</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="27"/>
+        <v>0.628649346</v>
+      </c>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C31">
+        <v>133</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>449</v>
+      </c>
+      <c r="F31" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" t="s">
+        <v>450</v>
+      </c>
+      <c r="H31">
+        <v>21</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="3"/>
+      <c r="L31" s="4"/>
+      <c r="O31">
+        <v>216</v>
+      </c>
+      <c r="P31">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.58787753799999998</v>
+      </c>
+      <c r="R31" s="4">
+        <v>240</v>
+      </c>
+      <c r="S31" s="3">
+        <v>19.86</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0.619677335</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="24"/>
+        <v>20.329999999999998</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="25"/>
+        <v>0.58787753799999998</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="26"/>
+        <v>19.86</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="27"/>
+        <v>0.619677335</v>
+      </c>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C32">
+        <v>134</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>451</v>
+      </c>
+      <c r="F32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" t="s">
+        <v>452</v>
+      </c>
+      <c r="H32">
+        <v>9</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="L32" s="4"/>
+      <c r="O32">
+        <v>233</v>
+      </c>
+      <c r="P32">
+        <v>11.89</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>0.30528675</v>
+      </c>
+      <c r="R32" s="4">
+        <v>250</v>
+      </c>
+      <c r="S32" s="3">
+        <v>11.49</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="24"/>
+        <v>11.89</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="25"/>
+        <v>0.30528675</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="26"/>
+        <v>11.49</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="27"/>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C33">
+        <v>135</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>451</v>
+      </c>
+      <c r="F33" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" t="s">
+        <v>452</v>
+      </c>
+      <c r="H33">
+        <v>15</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="3"/>
+      <c r="L33" s="4"/>
+      <c r="O33">
+        <v>231</v>
+      </c>
+      <c r="P33">
+        <v>11.77</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>0.30397368299999999</v>
+      </c>
+      <c r="R33" s="4">
+        <v>247</v>
+      </c>
+      <c r="S33" s="3">
+        <v>11.74</v>
+      </c>
+      <c r="T33" s="3">
+        <v>0.31432467291003424</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="24"/>
+        <v>11.77</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="25"/>
+        <v>0.30397368299999999</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="26"/>
+        <v>11.74</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="27"/>
+        <v>0.31432467291003424</v>
+      </c>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C34">
+        <v>136</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>451</v>
+      </c>
+      <c r="F34" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" t="s">
+        <v>452</v>
+      </c>
+      <c r="H34">
+        <v>21</v>
+      </c>
+      <c r="I34" s="4"/>
+      <c r="J34" s="3"/>
+      <c r="L34" s="4"/>
+      <c r="O34">
+        <v>216</v>
+      </c>
+      <c r="P34">
+        <v>11.79</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>0.29393876899999999</v>
+      </c>
+      <c r="R34" s="4">
+        <v>240</v>
+      </c>
+      <c r="S34" s="3">
+        <v>11.77</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0.30983866769659335</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="24"/>
+        <v>11.79</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="25"/>
+        <v>0.29393876899999999</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="26"/>
+        <v>11.77</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="27"/>
+        <v>0.30983866769659335</v>
+      </c>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>398</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
+        <v>398</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>427</v>
+      </c>
+      <c r="P36">
+        <v>44.62</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>10.24</v>
+      </c>
+      <c r="R36">
+        <v>714</v>
+      </c>
+      <c r="S36">
+        <v>46.18</v>
+      </c>
+      <c r="T36">
+        <v>11.23</v>
+      </c>
+      <c r="U36">
+        <f t="shared" ref="U36:U37" si="28">P36-J36</f>
+        <v>44.62</v>
+      </c>
+      <c r="V36">
+        <f t="shared" ref="V36:V37" si="29">IF(ISBLANK(I36), Q36, SQRT(Q36 ^ 2 / O36 + K36 ^ 2 / I36))</f>
+        <v>10.24</v>
+      </c>
+      <c r="W36">
+        <f t="shared" ref="W36:W37" si="30">S36 - M36</f>
+        <v>46.18</v>
+      </c>
+      <c r="X36">
+        <f t="shared" ref="X36:X37" si="31">IF(ISBLANK(I36), T36, SQRT(T36 ^ 2 / R36 + N36 ^ 2 / L36))</f>
+        <v>11.23</v>
+      </c>
+      <c r="AC36" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="2"/>
+      <c r="AS36" s="2"/>
+    </row>
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" t="s">
+        <v>397</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>399</v>
+      </c>
+      <c r="F37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" t="s">
+        <v>399</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>427</v>
+      </c>
+      <c r="P37">
+        <v>44.76</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="R37">
+        <v>714</v>
+      </c>
+      <c r="S37">
+        <v>46.17</v>
+      </c>
+      <c r="T37">
+        <v>8.49</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="28"/>
+        <v>44.76</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="29"/>
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="30"/>
+        <v>46.17</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="31"/>
+        <v>8.49</v>
+      </c>
+      <c r="AC37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="2"/>
+      <c r="AS37" s="2"/>
+    </row>
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" t="s">
+        <v>400</v>
+      </c>
+      <c r="C39">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>427</v>
+      </c>
+      <c r="P39">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>4.95</v>
+      </c>
+      <c r="R39">
+        <v>714</v>
+      </c>
+      <c r="S39">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="T39">
+        <v>5.35</v>
+      </c>
+      <c r="U39">
+        <f t="shared" ref="U39" si="32">P39-J39</f>
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="V39">
+        <f t="shared" ref="V39" si="33">IF(ISBLANK(I39), Q39, SQRT(Q39 ^ 2 / O39 + K39 ^ 2 / I39))</f>
+        <v>4.95</v>
+      </c>
+      <c r="W39">
+        <f t="shared" ref="W39" si="34">S39 - M39</f>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="X39">
+        <f t="shared" ref="X39" si="35">IF(ISBLANK(I39), T39, SQRT(T39 ^ 2 / R39 + N39 ^ 2 / L39))</f>
+        <v>5.35</v>
+      </c>
+      <c r="AC39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AS39" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{AA793D3B-DA33-48DD-81B4-9E7D3BBE01F6}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{952D37A7-DFC2-4953-8629-C96882F5A7E8}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{A4270B2A-17AE-44F6-8CEF-964EB64EE370}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{1A6A7C97-E3AB-4DDB-B435-B3C510066A02}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{771F1A4C-0C5E-43CD-AC07-72908B92C7CA}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{F1F3B9AC-A222-4A00-AFBD-51EAD94B6935}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{EBEE7AF0-E329-47FC-B2E3-67D2D9E97F0F}"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{282097B3-B51D-4942-BFFE-01A0DA72B895}"/>
+    <hyperlink ref="B12" r:id="rId9" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{F535AA40-BB0F-4F77-A5BF-0D3E6034BB41}"/>
+    <hyperlink ref="B14" r:id="rId10" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{AC9A96B7-F6F2-466A-BAAD-0A6A2F2AED55}"/>
+    <hyperlink ref="B15" r:id="rId11" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{B94DE2B4-3D8C-491D-B13D-4F7C51C14382}"/>
+    <hyperlink ref="B16" r:id="rId12" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?ga=1&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FJiao%20%282019%29%20Web%2Dbased%20versus%20home%2Dbased%20postnatal%20psychoeducational%20interventions%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{57A66675-D0BD-46CB-995C-52A12F62E7E5}"/>
+    <hyperlink ref="B22" r:id="rId13" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{E9242178-9012-483D-86FE-A82B4AB56358}"/>
+    <hyperlink ref="B23" r:id="rId14" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{278069AF-7FE7-4A87-A3BA-8127FC78FACC}"/>
+    <hyperlink ref="B24" r:id="rId15" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{228840F1-9DF0-4D2D-99D0-366E96EED3CE}"/>
+    <hyperlink ref="B25" r:id="rId16" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{0F7DAA86-F446-4D78-A6A8-0FD5FB9D48B4}"/>
+    <hyperlink ref="B26" r:id="rId17" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{1C7C1EBA-A3EB-4242-944C-138D62775EE9}"/>
+    <hyperlink ref="B27" r:id="rId18" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{02C8B752-CC38-493C-90C8-9168FE8DEC5E}"/>
+    <hyperlink ref="B29" r:id="rId19" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{C5C1A2A5-4C4D-40B3-BA8A-90F153844CE9}"/>
+    <hyperlink ref="B30" r:id="rId20" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{7821DAD1-029D-4E37-96E2-1641036E4EB7}"/>
+    <hyperlink ref="B31" r:id="rId21" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{D6B68A19-1780-4489-A61E-DA72234CE728}"/>
+    <hyperlink ref="B32" r:id="rId22" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{99DE361F-7257-4005-93D2-E58602B842BD}"/>
+    <hyperlink ref="B33" r:id="rId23" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{65224FBC-560A-4674-AD2B-4DFF9A343E19}"/>
+    <hyperlink ref="B34" r:id="rId24" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL%2FSawyer%20%282017%29%20Nurse%2DModerated%20Internet%2DBased%20Support%20for%20New%20Mothers%2D%20Non%2DInferiority%2C%20Randomized%20Controlled%20Trial%2Epdf&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FALL" xr:uid="{8BC1EA32-A939-4165-8114-EE09728147BD}"/>
+    <hyperlink ref="B36" r:id="rId25" display="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=7yiFtW&amp;cid=68fb9a55%2Db8f3%2D4c55%2Dae2a%2Df5cc58a16d15&amp;FolderCTID=0x012000C93EC9BF0A69C541B8FA2022D55A7013&amp;isAscending=false&amp;sortField=Modified&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FCiochon%202022%20Antenatal%20Classes%20in%20the%20Context%20of%20Prenatal%20Anxiety%20and%20Depression%20during%20the%20COVID%2D19%20Pandemic%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;q=Ciochon&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS&amp;parentview=7" xr:uid="{7BD64A97-AF7F-437E-ABE5-5555DF891E73}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId26"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0E04C6-D417-41CB-A789-3F3400450D65}">
   <dimension ref="A1:W38"/>
   <sheetViews>
@@ -18913,12 +21179,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f1c3b6d-7f32-4752-9b60-8760effeb2ab">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b77b1af8-43ce-437e-80a0-2a6bb447a677" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19153,20 +21421,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f1c3b6d-7f32-4752-9b60-8760effeb2ab">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b77b1af8-43ce-437e-80a0-2a6bb447a677" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C637C4C-9A48-4ADA-A1DE-A69ED46A1145}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B935DA7E-A5AF-431A-9EAB-82483DAFB6C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b77b1af8-43ce-437e-80a0-2a6bb447a677"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6f1c3b6d-7f32-4752-9b60-8760effeb2ab"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19191,18 +21466,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B935DA7E-A5AF-431A-9EAB-82483DAFB6C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C637C4C-9A48-4ADA-A1DE-A69ED46A1145}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b77b1af8-43ce-437e-80a0-2a6bb447a677"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6f1c3b6d-7f32-4752-9b60-8760effeb2ab"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Additional sensitivity analyses; int vs time analysis
</commit_message>
<xml_diff>
--- a/data/data_extraction_te_20230205.xlsx
+++ b/data/data_extraction_te_20230205.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared Documents/General/ONLINE PARENTING SR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7120374D-4FC4-4495-9A5D-BF509F7F36D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C05657F-C13A-424B-BD0C-01FF7CDABAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2550" uniqueCount="472">
   <si>
     <t>study</t>
   </si>
@@ -1501,9 +1501,6 @@
   </si>
   <si>
     <t>https://latrobeuni.sharepoint.com/teams/O365-OnlineParentingSR/Shared%20Documents/Forms/AllItems.aspx?csf=1&amp;web=1&amp;e=7yiFtW&amp;cid=68fb9a55%2Db8f3%2D4c55%2Dae2a%2Df5cc58a16d15&amp;FolderCTID=0x012000C93EC9BF0A69C541B8FA2022D55A7013&amp;isAscending=false&amp;sortField=Modified&amp;id=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS%2FZhang%202023%20Effectiveness%20of%20Digital%20Guided%20Self%2Dhelp%20Mindfulness%20Training%20During%20Pregnancy%20on%20Maternal%20Psychological%2Epdf&amp;viewid=4fbd683f%2Dbc81%2D4ccf%2Da362%2D5e25f0a3d027&amp;q=Zhang&amp;parent=%2Fteams%2FO365%2DOnlineParentingSR%2FShared%20Documents%2FGeneral%2FONLINE%20PARENTING%20SR%2FINCLUDED%20PAPERS&amp;parentview=7</t>
-  </si>
-  <si>
-    <t>In-person</t>
   </si>
   <si>
     <t>Change from baseline reported</t>
@@ -7735,7 +7732,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F3" sqref="F3"/>
+      <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -9622,7 +9619,7 @@
         <v>400</v>
       </c>
       <c r="F23" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="G23" t="s">
         <v>53</v>
@@ -10898,7 +10895,7 @@
         <v>1</v>
       </c>
       <c r="AF39" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="40" spans="1:47">
@@ -11569,7 +11566,7 @@
         <v>200</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -11873,7 +11870,7 @@
         <v>1</v>
       </c>
       <c r="AF51" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="52" spans="1:47">
@@ -13649,7 +13646,7 @@
         <v>202</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C77">
         <v>76</v>
@@ -13739,7 +13736,7 @@
         <v>202</v>
       </c>
       <c r="B78" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C78">
         <v>77</v>
@@ -13829,7 +13826,7 @@
         <v>178</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C79">
         <v>78</v>
@@ -14073,7 +14070,7 @@
         <v>164</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C82">
         <v>81</v>
@@ -14147,7 +14144,7 @@
         <v>164</v>
       </c>
       <c r="B83" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C83">
         <v>82</v>
@@ -14221,7 +14218,7 @@
         <v>164</v>
       </c>
       <c r="B84" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C84">
         <v>83</v>
@@ -14295,7 +14292,7 @@
         <v>51</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C85">
         <v>84</v>
@@ -14310,13 +14307,13 @@
         <v>401</v>
       </c>
       <c r="G85" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H85" t="s">
         <v>338</v>
       </c>
       <c r="I85" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J85">
         <v>5</v>
@@ -14388,7 +14385,7 @@
         <v>51</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C86">
         <v>85</v>
@@ -14403,13 +14400,13 @@
         <v>401</v>
       </c>
       <c r="G86" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H86" t="s">
         <v>338</v>
       </c>
       <c r="I86" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J86">
         <v>5</v>
@@ -14481,7 +14478,7 @@
         <v>92</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C87">
         <v>86</v>
@@ -14496,7 +14493,7 @@
         <v>401</v>
       </c>
       <c r="G87" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H87" t="s">
         <v>338</v>
@@ -14565,7 +14562,7 @@
         <v>92</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C88">
         <v>87</v>
@@ -14580,7 +14577,7 @@
         <v>401</v>
       </c>
       <c r="G88" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H88" t="s">
         <v>338</v>
@@ -14649,7 +14646,7 @@
         <v>92</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C89">
         <v>88</v>
@@ -14664,7 +14661,7 @@
         <v>401</v>
       </c>
       <c r="G89" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H89" t="s">
         <v>338</v>
@@ -14733,7 +14730,7 @@
         <v>103</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C90">
         <v>89</v>
@@ -14748,7 +14745,7 @@
         <v>406</v>
       </c>
       <c r="G90" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H90" t="s">
         <v>338</v>
@@ -14799,7 +14796,7 @@
         <v>196</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C91">
         <v>90</v>
@@ -14814,7 +14811,7 @@
         <v>401</v>
       </c>
       <c r="G91" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H91" t="s">
         <v>338</v>
@@ -14868,7 +14865,7 @@
         <v>196</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C92">
         <v>91</v>
@@ -14883,7 +14880,7 @@
         <v>401</v>
       </c>
       <c r="G92" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H92" t="s">
         <v>338</v>
@@ -14937,7 +14934,7 @@
         <v>186</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C93">
         <v>92</v>
@@ -15006,10 +15003,10 @@
     </row>
     <row r="94" spans="1:47">
       <c r="A94" t="s">
+        <v>435</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>437</v>
       </c>
       <c r="C94">
         <v>93</v>
@@ -15024,7 +15021,7 @@
         <v>406</v>
       </c>
       <c r="G94" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H94" t="s">
         <v>338</v>
@@ -15628,7 +15625,7 @@
         <v>164</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C102">
         <v>101</v>
@@ -15649,7 +15646,7 @@
         <v>160</v>
       </c>
       <c r="I102" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J102">
         <v>9</v>
@@ -15707,7 +15704,7 @@
         <v>164</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C103">
         <v>102</v>
@@ -15728,7 +15725,7 @@
         <v>160</v>
       </c>
       <c r="I103" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J103">
         <v>15</v>
@@ -15792,7 +15789,7 @@
         <v>164</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C104">
         <v>103</v>
@@ -15813,7 +15810,7 @@
         <v>160</v>
       </c>
       <c r="I104" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J104">
         <v>21</v>
@@ -15877,7 +15874,7 @@
         <v>164</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C105">
         <v>104</v>
@@ -15898,7 +15895,7 @@
         <v>160</v>
       </c>
       <c r="I105" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J105">
         <v>9</v>
@@ -15956,7 +15953,7 @@
         <v>164</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C106">
         <v>105</v>
@@ -15977,7 +15974,7 @@
         <v>160</v>
       </c>
       <c r="I106" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J106">
         <v>15</v>
@@ -16035,7 +16032,7 @@
         <v>164</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C107">
         <v>106</v>
@@ -16056,7 +16053,7 @@
         <v>160</v>
       </c>
       <c r="I107" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J107">
         <v>21</v>
@@ -16198,7 +16195,7 @@
         <v>160</v>
       </c>
       <c r="I109" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J109">
         <v>1</v>
@@ -16453,7 +16450,7 @@
         <v>202</v>
       </c>
       <c r="B113" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C113">
         <v>112</v>
@@ -16537,7 +16534,7 @@
         <v>202</v>
       </c>
       <c r="B114" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C114">
         <v>113</v>
@@ -16621,7 +16618,7 @@
         <v>92</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -16636,13 +16633,13 @@
         <v>401</v>
       </c>
       <c r="G115" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H115" t="s">
         <v>94</v>
       </c>
       <c r="I115" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J115">
         <v>3</v>
@@ -16708,7 +16705,7 @@
         <v>92</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C116">
         <v>115</v>
@@ -16723,13 +16720,13 @@
         <v>401</v>
       </c>
       <c r="G116" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H116" t="s">
         <v>94</v>
       </c>
       <c r="I116" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J116">
         <v>6</v>
@@ -16795,7 +16792,7 @@
         <v>92</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C117">
         <v>116</v>
@@ -16810,13 +16807,13 @@
         <v>401</v>
       </c>
       <c r="G117" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H117" t="s">
         <v>94</v>
       </c>
       <c r="I117" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J117">
         <v>12</v>
@@ -16882,7 +16879,7 @@
         <v>92</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C118">
         <v>117</v>
@@ -16897,13 +16894,13 @@
         <v>401</v>
       </c>
       <c r="G118" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H118" t="s">
         <v>94</v>
       </c>
       <c r="I118" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J118">
         <v>3</v>
@@ -16969,7 +16966,7 @@
         <v>92</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C119">
         <v>118</v>
@@ -16984,13 +16981,13 @@
         <v>401</v>
       </c>
       <c r="G119" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H119" t="s">
         <v>94</v>
       </c>
       <c r="I119" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J119">
         <v>6</v>
@@ -17056,7 +17053,7 @@
         <v>92</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C120">
         <v>119</v>
@@ -17071,13 +17068,13 @@
         <v>401</v>
       </c>
       <c r="G120" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H120" t="s">
         <v>94</v>
       </c>
       <c r="I120" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J120">
         <v>12</v>
@@ -17149,7 +17146,7 @@
         <v>92</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C121">
         <v>120</v>
@@ -17164,13 +17161,13 @@
         <v>401</v>
       </c>
       <c r="G121" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H121" t="s">
         <v>94</v>
       </c>
       <c r="I121" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J121">
         <v>3</v>
@@ -17242,7 +17239,7 @@
         <v>92</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C122">
         <v>121</v>
@@ -17257,13 +17254,13 @@
         <v>401</v>
       </c>
       <c r="G122" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H122" t="s">
         <v>94</v>
       </c>
       <c r="I122" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J122">
         <v>6</v>
@@ -17329,7 +17326,7 @@
         <v>92</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C123">
         <v>122</v>
@@ -17344,13 +17341,13 @@
         <v>401</v>
       </c>
       <c r="G123" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H123" t="s">
         <v>94</v>
       </c>
       <c r="I123" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J123">
         <v>12</v>
@@ -17416,7 +17413,7 @@
         <v>103</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C124">
         <v>123</v>
@@ -17482,7 +17479,7 @@
         <v>69</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C125">
         <v>124</v>
@@ -17503,7 +17500,7 @@
         <v>94</v>
       </c>
       <c r="I125" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J125">
         <v>0</v>
@@ -17551,7 +17548,7 @@
         <v>69</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C126">
         <v>125</v>
@@ -17620,7 +17617,7 @@
         <v>111</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C127">
         <v>126</v>
@@ -17641,7 +17638,7 @@
         <v>94</v>
       </c>
       <c r="I127" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J127">
         <v>0</v>
@@ -17689,7 +17686,7 @@
         <v>111</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C128">
         <v>127</v>
@@ -17710,7 +17707,7 @@
         <v>94</v>
       </c>
       <c r="I128" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J128">
         <v>0</v>
@@ -17764,7 +17761,7 @@
         <v>71</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C129">
         <v>128</v>
@@ -17986,7 +17983,7 @@
         <v>164</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C132">
         <v>131</v>
@@ -18001,13 +17998,13 @@
         <v>401</v>
       </c>
       <c r="G132" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H132" t="s">
         <v>94</v>
       </c>
       <c r="I132" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J132">
         <v>9</v>
@@ -18065,7 +18062,7 @@
         <v>164</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C133">
         <v>132</v>
@@ -18080,13 +18077,13 @@
         <v>401</v>
       </c>
       <c r="G133" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H133" t="s">
         <v>94</v>
       </c>
       <c r="I133" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J133">
         <v>15</v>
@@ -18144,7 +18141,7 @@
         <v>164</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C134">
         <v>133</v>
@@ -18159,13 +18156,13 @@
         <v>401</v>
       </c>
       <c r="G134" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H134" t="s">
         <v>94</v>
       </c>
       <c r="I134" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J134">
         <v>21</v>
@@ -18223,7 +18220,7 @@
         <v>164</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C135">
         <v>134</v>
@@ -18238,13 +18235,13 @@
         <v>401</v>
       </c>
       <c r="G135" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H135" t="s">
         <v>94</v>
       </c>
       <c r="I135" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J135">
         <v>9</v>
@@ -18302,7 +18299,7 @@
         <v>164</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C136">
         <v>135</v>
@@ -18317,13 +18314,13 @@
         <v>401</v>
       </c>
       <c r="G136" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H136" t="s">
         <v>94</v>
       </c>
       <c r="I136" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J136">
         <v>15</v>
@@ -18381,7 +18378,7 @@
         <v>164</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C137">
         <v>136</v>
@@ -18396,13 +18393,13 @@
         <v>401</v>
       </c>
       <c r="G137" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H137" t="s">
         <v>94</v>
       </c>
       <c r="I137" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J137">
         <v>21</v>
@@ -18460,7 +18457,7 @@
         <v>202</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C138">
         <v>137</v>
@@ -18547,7 +18544,7 @@
         <v>202</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C139">
         <v>138</v>
@@ -18634,7 +18631,7 @@
         <v>200</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C140">
         <v>139</v>
@@ -19708,7 +19705,7 @@
         <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C18">
         <v>81</v>
@@ -19773,7 +19770,7 @@
         <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C19">
         <v>82</v>
@@ -19838,7 +19835,7 @@
         <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C20">
         <v>83</v>
@@ -19903,7 +19900,7 @@
         <v>164</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C22">
         <v>101</v>
@@ -19918,7 +19915,7 @@
         <v>160</v>
       </c>
       <c r="G22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H22">
         <v>9</v>
@@ -19979,7 +19976,7 @@
         <v>164</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C23">
         <v>102</v>
@@ -19994,7 +19991,7 @@
         <v>160</v>
       </c>
       <c r="G23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H23">
         <v>15</v>
@@ -20055,7 +20052,7 @@
         <v>164</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C24">
         <v>103</v>
@@ -20070,7 +20067,7 @@
         <v>160</v>
       </c>
       <c r="G24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H24">
         <v>21</v>
@@ -20131,7 +20128,7 @@
         <v>164</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C25">
         <v>104</v>
@@ -20146,7 +20143,7 @@
         <v>160</v>
       </c>
       <c r="G25" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H25">
         <v>9</v>
@@ -20207,7 +20204,7 @@
         <v>164</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C26">
         <v>105</v>
@@ -20222,7 +20219,7 @@
         <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H26">
         <v>15</v>
@@ -20283,7 +20280,7 @@
         <v>164</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C27">
         <v>106</v>
@@ -20298,7 +20295,7 @@
         <v>160</v>
       </c>
       <c r="G27" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H27">
         <v>21</v>
@@ -20359,7 +20356,7 @@
         <v>164</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C29">
         <v>131</v>
@@ -20368,13 +20365,13 @@
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F29" t="s">
         <v>94</v>
       </c>
       <c r="G29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H29">
         <v>9</v>
@@ -20429,7 +20426,7 @@
         <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C30">
         <v>132</v>
@@ -20438,13 +20435,13 @@
         <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F30" t="s">
         <v>94</v>
       </c>
       <c r="G30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H30">
         <v>15</v>
@@ -20499,7 +20496,7 @@
         <v>164</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C31">
         <v>133</v>
@@ -20508,13 +20505,13 @@
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F31" t="s">
         <v>94</v>
       </c>
       <c r="G31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H31">
         <v>21</v>
@@ -20569,7 +20566,7 @@
         <v>164</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C32">
         <v>134</v>
@@ -20578,13 +20575,13 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F32" t="s">
         <v>94</v>
       </c>
       <c r="G32" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H32">
         <v>9</v>
@@ -20639,7 +20636,7 @@
         <v>164</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C33">
         <v>135</v>
@@ -20648,13 +20645,13 @@
         <v>22</v>
       </c>
       <c r="E33" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F33" t="s">
         <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H33">
         <v>15</v>
@@ -20709,7 +20706,7 @@
         <v>164</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C34">
         <v>136</v>
@@ -20718,13 +20715,13 @@
         <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F34" t="s">
         <v>94</v>
       </c>
       <c r="G34" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H34">
         <v>21</v>
@@ -21020,82 +21017,82 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="16" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="G1" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="10"/>
       <c r="M1" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N1" s="17"/>
       <c r="Q1" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="R1" s="17"/>
       <c r="S1" s="17"/>
       <c r="U1" s="16" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="V1" s="16"/>
       <c r="W1" s="16"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K2" s="1"/>
       <c r="M2" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>472</v>
-      </c>
       <c r="R2" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="U2" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>465</v>
-      </c>
       <c r="W2" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -22041,12 +22038,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f1c3b6d-7f32-4752-9b60-8760effeb2ab">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b77b1af8-43ce-437e-80a0-2a6bb447a677" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22281,18 +22280,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f1c3b6d-7f32-4752-9b60-8760effeb2ab">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b77b1af8-43ce-437e-80a0-2a6bb447a677" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C637C4C-9A48-4ADA-A1DE-A69ED46A1145}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B935DA7E-A5AF-431A-9EAB-82483DAFB6C2}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22300,5 +22297,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B935DA7E-A5AF-431A-9EAB-82483DAFB6C2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C637C4C-9A48-4ADA-A1DE-A69ED46A1145}"/>
 </file>
</xml_diff>